<commit_message>
added minor comments + updated package doc
</commit_message>
<xml_diff>
--- a/tables/input/output_processed_table.xlsx
+++ b/tables/input/output_processed_table.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:AD11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -435,7 +435,7 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>AF.kN.m</t>
+          <t>P.kN.m</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
@@ -470,12 +470,42 @@
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
+          <t>gamma</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
           <t>Ned</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>selected_member_size</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>check1.kN</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>check2.kN</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>check3.kN</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>N_ch_Ed</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>final_check</t>
         </is>
       </c>
     </row>
@@ -553,12 +583,30 @@
         <v>10</v>
       </c>
       <c r="W2">
-        <v>2269</v>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>457 x 152 x 74</t>
-        </is>
+        <v>1.35</v>
+      </c>
+      <c r="X2">
+        <v>2542</v>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>686 x 254 x 125</t>
+        </is>
+      </c>
+      <c r="Z2">
+        <v>8489</v>
+      </c>
+      <c r="AA2">
+        <v>10666</v>
+      </c>
+      <c r="AB2">
+        <v>5430</v>
+      </c>
+      <c r="AC2">
+        <v>1278</v>
+      </c>
+      <c r="AD2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -635,12 +683,30 @@
         <v>10</v>
       </c>
       <c r="W3">
-        <v>2104</v>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>457 x 152 x 60</t>
-        </is>
+        <v>1.35</v>
+      </c>
+      <c r="X3">
+        <v>2424</v>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>686 x 254 x 125</t>
+        </is>
+      </c>
+      <c r="Z3">
+        <v>9753</v>
+      </c>
+      <c r="AA3">
+        <v>10893</v>
+      </c>
+      <c r="AB3">
+        <v>5430</v>
+      </c>
+      <c r="AC3">
+        <v>1216</v>
+      </c>
+      <c r="AD3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -717,12 +783,30 @@
         <v>10</v>
       </c>
       <c r="W4">
-        <v>3549</v>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>610 x 229 x 101</t>
-        </is>
+        <v>1.35</v>
+      </c>
+      <c r="X4">
+        <v>3638</v>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>686 x 254 x 125</t>
+        </is>
+      </c>
+      <c r="Z4">
+        <v>8489</v>
+      </c>
+      <c r="AA4">
+        <v>10666</v>
+      </c>
+      <c r="AB4">
+        <v>5430</v>
+      </c>
+      <c r="AC4">
+        <v>1828</v>
+      </c>
+      <c r="AD4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -799,12 +883,30 @@
         <v>10</v>
       </c>
       <c r="W5">
-        <v>3341</v>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>610 x 178 x 92</t>
-        </is>
+        <v>1.35</v>
+      </c>
+      <c r="X5">
+        <v>3430</v>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>686 x 254 x 125</t>
+        </is>
+      </c>
+      <c r="Z5">
+        <v>9753</v>
+      </c>
+      <c r="AA5">
+        <v>10893</v>
+      </c>
+      <c r="AB5">
+        <v>5430</v>
+      </c>
+      <c r="AC5">
+        <v>1721</v>
+      </c>
+      <c r="AD5" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -881,12 +983,30 @@
         <v>10</v>
       </c>
       <c r="W6">
-        <v>8036</v>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>914 x 305 x 224</t>
-        </is>
+        <v>1.35</v>
+      </c>
+      <c r="X6">
+        <v>8260</v>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>838 x 292 x 226</t>
+        </is>
+      </c>
+      <c r="Z6">
+        <v>17221</v>
+      </c>
+      <c r="AA6">
+        <v>19386</v>
+      </c>
+      <c r="AB6">
+        <v>9959</v>
+      </c>
+      <c r="AC6">
+        <v>4152</v>
+      </c>
+      <c r="AD6" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -963,12 +1083,30 @@
         <v>10</v>
       </c>
       <c r="W7">
-        <v>7572</v>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>762 x 267 x 197</t>
-        </is>
+        <v>1.35</v>
+      </c>
+      <c r="X7">
+        <v>7787</v>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>1016 x 305 x 222</t>
+        </is>
+      </c>
+      <c r="Z7">
+        <v>18434</v>
+      </c>
+      <c r="AA7">
+        <v>19388</v>
+      </c>
+      <c r="AB7">
+        <v>9716</v>
+      </c>
+      <c r="AC7">
+        <v>3908</v>
+      </c>
+      <c r="AD7" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -1045,12 +1183,30 @@
         <v>10</v>
       </c>
       <c r="W8">
-        <v>7955</v>
-      </c>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>1016 x 305 x 222</t>
-        </is>
+        <v>1.35</v>
+      </c>
+      <c r="X8">
+        <v>8176</v>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>914 x 305 x 224</t>
+        </is>
+      </c>
+      <c r="Z8">
+        <v>17339</v>
+      </c>
+      <c r="AA8">
+        <v>19185</v>
+      </c>
+      <c r="AB8">
+        <v>9854</v>
+      </c>
+      <c r="AC8">
+        <v>4109</v>
+      </c>
+      <c r="AD8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -1127,12 +1283,30 @@
         <v>10</v>
       </c>
       <c r="W9">
-        <v>7495</v>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>762 x 267 x 197</t>
-        </is>
+        <v>1.35</v>
+      </c>
+      <c r="X9">
+        <v>7709</v>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>1016 x 305 x 222</t>
+        </is>
+      </c>
+      <c r="Z9">
+        <v>18434</v>
+      </c>
+      <c r="AA9">
+        <v>19388</v>
+      </c>
+      <c r="AB9">
+        <v>9716</v>
+      </c>
+      <c r="AC9">
+        <v>3869</v>
+      </c>
+      <c r="AD9" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1209,12 +1383,30 @@
         <v>10</v>
       </c>
       <c r="W10">
-        <v>9494</v>
-      </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>914 x 305 x 253</t>
-        </is>
+        <v>1.35</v>
+      </c>
+      <c r="X10">
+        <v>9761</v>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>1016 x 305 x 272</t>
+        </is>
+      </c>
+      <c r="Z10">
+        <v>21566</v>
+      </c>
+      <c r="AA10">
+        <v>23277</v>
+      </c>
+      <c r="AB10">
+        <v>11963</v>
+      </c>
+      <c r="AC10">
+        <v>4906</v>
+      </c>
+      <c r="AD10" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -1291,12 +1483,30 @@
         <v>10</v>
       </c>
       <c r="W11">
-        <v>8946</v>
-      </c>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>914 x 305 x 238</t>
-        </is>
+        <v>1.35</v>
+      </c>
+      <c r="X11">
+        <v>9203</v>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>1016 x 305 x 249</t>
+        </is>
+      </c>
+      <c r="Z11">
+        <v>20714</v>
+      </c>
+      <c r="AA11">
+        <v>21718</v>
+      </c>
+      <c r="AB11">
+        <v>10909</v>
+      </c>
+      <c r="AC11">
+        <v>4618</v>
+      </c>
+      <c r="AD11" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug due to new version of readxl
</commit_message>
<xml_diff>
--- a/tables/input/output_processed_table.xlsx
+++ b/tables/input/output_processed_table.xlsx
@@ -678,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="P2">
-        <v>247</v>
+        <v>686</v>
       </c>
       <c r="Q2">
         <v>50</v>
@@ -706,51 +706,51 @@
         <v>1.35</v>
       </c>
       <c r="X2">
-        <v>150</v>
+        <v>345</v>
       </c>
       <c r="Y2">
-        <v>1180</v>
+        <v>3208</v>
       </c>
       <c r="Z2">
-        <v>590</v>
+        <v>1604</v>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>305 x 102 x 28</t>
+          <t>406 x 178 x 54</t>
         </is>
       </c>
       <c r="AB2">
         <v>355</v>
       </c>
       <c r="AC2">
-        <v>2549</v>
+        <v>4899</v>
       </c>
       <c r="AD2">
-        <v>712</v>
+        <v>2481</v>
       </c>
       <c r="AE2">
-        <v>1.89</v>
+        <v>1.41</v>
       </c>
       <c r="AF2">
         <v>0.21</v>
       </c>
       <c r="AG2">
-        <v>0.25</v>
+        <v>0.42</v>
       </c>
       <c r="AH2">
-        <v>629</v>
+        <v>2035</v>
       </c>
       <c r="AI2">
         <v>355</v>
       </c>
       <c r="AJ2">
-        <v>2549</v>
+        <v>4899</v>
       </c>
       <c r="AK2">
-        <v>179500</v>
+        <v>345000</v>
       </c>
       <c r="AL2">
-        <v>23810</v>
+        <v>45763</v>
       </c>
       <c r="AM2">
         <v>0.33</v>
@@ -762,40 +762,40 @@
         <v>0.97</v>
       </c>
       <c r="AP2">
-        <v>2475</v>
+        <v>4757</v>
       </c>
       <c r="AQ2">
         <v>355</v>
       </c>
       <c r="AR2">
-        <v>1274</v>
+        <v>2450</v>
       </c>
       <c r="AS2">
-        <v>3213</v>
+        <v>21141</v>
       </c>
       <c r="AT2">
-        <v>0.63</v>
+        <v>0.34</v>
       </c>
       <c r="AU2">
         <v>0.21</v>
       </c>
       <c r="AV2">
-        <v>0.88</v>
+        <v>0.97</v>
       </c>
       <c r="AW2">
-        <v>1119</v>
+        <v>2371</v>
       </c>
       <c r="AX2">
         <v>169281363</v>
       </c>
       <c r="AY2">
-        <v>23810</v>
+        <v>45763</v>
       </c>
       <c r="AZ2">
-        <v>231355</v>
+        <v>42</v>
       </c>
       <c r="BA2">
-        <v>297</v>
+        <v>806</v>
       </c>
       <c r="BB2" t="b">
         <v>1</v>
@@ -850,7 +850,7 @@
         <v>1</v>
       </c>
       <c r="P3">
-        <v>247</v>
+        <v>686</v>
       </c>
       <c r="Q3">
         <v>50</v>
@@ -878,51 +878,51 @@
         <v>1.35</v>
       </c>
       <c r="X3">
-        <v>142</v>
+        <v>286</v>
       </c>
       <c r="Y3">
-        <v>1114</v>
+        <v>2984</v>
       </c>
       <c r="Z3">
-        <v>557</v>
+        <v>1492</v>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>203 x 133 x 30</t>
+          <t>356 x 171 x 45</t>
         </is>
       </c>
       <c r="AB3">
         <v>355</v>
       </c>
       <c r="AC3">
-        <v>2712</v>
+        <v>4068</v>
       </c>
       <c r="AD3">
-        <v>742</v>
+        <v>3096</v>
       </c>
       <c r="AE3">
-        <v>1.91</v>
+        <v>1.15</v>
       </c>
       <c r="AF3">
         <v>0.21</v>
       </c>
       <c r="AG3">
-        <v>0.24</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AH3">
-        <v>657</v>
+        <v>2298</v>
       </c>
       <c r="AI3">
         <v>355</v>
       </c>
       <c r="AJ3">
-        <v>2712</v>
+        <v>4068</v>
       </c>
       <c r="AK3">
-        <v>191000</v>
+        <v>286500</v>
       </c>
       <c r="AL3">
-        <v>48873</v>
+        <v>73309</v>
       </c>
       <c r="AM3">
         <v>0.24</v>
@@ -934,40 +934,40 @@
         <v>0.99</v>
       </c>
       <c r="AP3">
-        <v>2691</v>
+        <v>4036</v>
       </c>
       <c r="AQ3">
         <v>355</v>
       </c>
       <c r="AR3">
-        <v>1356</v>
+        <v>2034</v>
       </c>
       <c r="AS3">
-        <v>7980</v>
+        <v>16809</v>
       </c>
       <c r="AT3">
-        <v>0.41</v>
+        <v>0.35</v>
       </c>
       <c r="AU3">
         <v>0.21</v>
       </c>
       <c r="AV3">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="AW3">
-        <v>1288</v>
+        <v>1965</v>
       </c>
       <c r="AX3">
         <v>169281363</v>
       </c>
       <c r="AY3">
-        <v>48873</v>
+        <v>73309</v>
       </c>
       <c r="AZ3">
-        <v>231355</v>
+        <v>27</v>
       </c>
       <c r="BA3">
-        <v>280</v>
+        <v>749</v>
       </c>
       <c r="BB3" t="b">
         <v>1</v>
@@ -1022,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="P4">
-        <v>436</v>
+        <v>1164</v>
       </c>
       <c r="Q4">
         <v>50</v>
@@ -1050,51 +1050,51 @@
         <v>1.35</v>
       </c>
       <c r="Y4">
-        <v>3638</v>
+        <v>9712</v>
       </c>
       <c r="Z4">
-        <v>1819</v>
+        <v>4856</v>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>406 x 178 x 60</t>
+          <t>686 x 254 x 140</t>
         </is>
       </c>
       <c r="AB4">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AC4">
-        <v>5432</v>
+        <v>12282</v>
       </c>
       <c r="AD4">
-        <v>2865</v>
+        <v>18040</v>
       </c>
       <c r="AE4">
-        <v>1.38</v>
+        <v>0.83</v>
       </c>
       <c r="AF4">
         <v>0.21</v>
       </c>
       <c r="AG4">
-        <v>0.43</v>
+        <v>0.78</v>
       </c>
       <c r="AH4">
-        <v>2332</v>
+        <v>9593</v>
       </c>
       <c r="AI4">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AJ4">
-        <v>5432</v>
+        <v>12282</v>
       </c>
       <c r="AK4">
-        <v>382500</v>
+        <v>890000</v>
       </c>
       <c r="AL4">
-        <v>50738</v>
+        <v>118056</v>
       </c>
       <c r="AM4">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
       <c r="AN4">
         <v>0.21</v>
@@ -1103,40 +1103,40 @@
         <v>0.97</v>
       </c>
       <c r="AP4">
-        <v>5274</v>
+        <v>11940</v>
       </c>
       <c r="AQ4">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AR4">
-        <v>2716</v>
+        <v>6141</v>
       </c>
       <c r="AS4">
-        <v>24871</v>
+        <v>107362</v>
       </c>
       <c r="AT4">
-        <v>0.33</v>
+        <v>0.24</v>
       </c>
       <c r="AU4">
         <v>0.21</v>
       </c>
       <c r="AV4">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
       <c r="AW4">
-        <v>2635</v>
+        <v>6088</v>
       </c>
       <c r="AX4">
         <v>169281363</v>
       </c>
       <c r="AY4">
-        <v>50738</v>
+        <v>118056</v>
       </c>
       <c r="AZ4">
-        <v>231355</v>
+        <v>127</v>
       </c>
       <c r="BA4">
-        <v>914</v>
+        <v>2441</v>
       </c>
       <c r="BB4" t="b">
         <v>1</v>
@@ -1191,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="P5">
-        <v>436</v>
+        <v>1164</v>
       </c>
       <c r="Q5">
         <v>50</v>
@@ -1219,51 +1219,51 @@
         <v>1.35</v>
       </c>
       <c r="Y5">
-        <v>3430</v>
+        <v>9156</v>
       </c>
       <c r="Z5">
-        <v>1715</v>
+        <v>4578</v>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>356 x 171 x 51</t>
+          <t>610 x 229 x 125</t>
         </is>
       </c>
       <c r="AB5">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AC5">
-        <v>4608</v>
+        <v>10971</v>
       </c>
       <c r="AD5">
-        <v>3608</v>
+        <v>25230</v>
       </c>
       <c r="AE5">
-        <v>1.13</v>
+        <v>0.66</v>
       </c>
       <c r="AF5">
         <v>0.21</v>
       </c>
       <c r="AG5">
-        <v>0.58</v>
+        <v>0.87</v>
       </c>
       <c r="AH5">
-        <v>2652</v>
+        <v>9501</v>
       </c>
       <c r="AI5">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AJ5">
-        <v>4608</v>
+        <v>10971</v>
       </c>
       <c r="AK5">
-        <v>324500</v>
+        <v>795000</v>
       </c>
       <c r="AL5">
-        <v>83033</v>
+        <v>203424</v>
       </c>
       <c r="AM5">
-        <v>0.24</v>
+        <v>0.23</v>
       </c>
       <c r="AN5">
         <v>0.21</v>
@@ -1272,40 +1272,40 @@
         <v>0.99</v>
       </c>
       <c r="AP5">
-        <v>4572</v>
+        <v>10893</v>
       </c>
       <c r="AQ5">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AR5">
-        <v>2304</v>
+        <v>5486</v>
       </c>
       <c r="AS5">
-        <v>20063</v>
+        <v>81454</v>
       </c>
       <c r="AT5">
-        <v>0.34</v>
+        <v>0.26</v>
       </c>
       <c r="AU5">
         <v>0.21</v>
       </c>
       <c r="AV5">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
       <c r="AW5">
-        <v>2231</v>
+        <v>5413</v>
       </c>
       <c r="AX5">
         <v>169281363</v>
       </c>
       <c r="AY5">
-        <v>83033</v>
+        <v>203424</v>
       </c>
       <c r="AZ5">
-        <v>231355</v>
+        <v>84</v>
       </c>
       <c r="BA5">
-        <v>861</v>
+        <v>2297</v>
       </c>
       <c r="BB5" t="b">
         <v>1</v>
@@ -1360,7 +1360,7 @@
         <v>1</v>
       </c>
       <c r="P6">
-        <v>990</v>
+        <v>1962</v>
       </c>
       <c r="Q6">
         <v>50</v>
@@ -1388,48 +1388,48 @@
         <v>1.35</v>
       </c>
       <c r="Y6">
-        <v>8260</v>
+        <v>16368</v>
       </c>
       <c r="Z6">
-        <v>4130</v>
+        <v>8184</v>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>686 x 254 x 125</t>
+          <t>914 x 305 x 224</t>
         </is>
       </c>
       <c r="AB6">
         <v>345</v>
       </c>
       <c r="AC6">
-        <v>10971</v>
+        <v>19734</v>
       </c>
       <c r="AD6">
-        <v>15652</v>
+        <v>49875</v>
       </c>
       <c r="AE6">
-        <v>0.84</v>
+        <v>0.63</v>
       </c>
       <c r="AF6">
         <v>0.21</v>
       </c>
       <c r="AG6">
-        <v>0.77</v>
+        <v>0.88</v>
       </c>
       <c r="AH6">
-        <v>8489</v>
+        <v>17339</v>
       </c>
       <c r="AI6">
         <v>345</v>
       </c>
       <c r="AJ6">
-        <v>10971</v>
+        <v>19734</v>
       </c>
       <c r="AK6">
-        <v>795000</v>
+        <v>1430000</v>
       </c>
       <c r="AL6">
-        <v>105455</v>
+        <v>189686</v>
       </c>
       <c r="AM6">
         <v>0.32</v>
@@ -1441,40 +1441,40 @@
         <v>0.97</v>
       </c>
       <c r="AP6">
-        <v>10666</v>
+        <v>19185</v>
       </c>
       <c r="AQ6">
         <v>345</v>
       </c>
       <c r="AR6">
-        <v>5486</v>
+        <v>9867</v>
       </c>
       <c r="AS6">
-        <v>90781</v>
+        <v>232133</v>
       </c>
       <c r="AT6">
-        <v>0.25</v>
+        <v>0.21</v>
       </c>
       <c r="AU6">
         <v>0.21</v>
       </c>
       <c r="AV6">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="AW6">
-        <v>5430</v>
+        <v>9854</v>
       </c>
       <c r="AX6">
         <v>169281363</v>
       </c>
       <c r="AY6">
-        <v>105455</v>
+        <v>189686</v>
       </c>
       <c r="AZ6">
-        <v>231355</v>
+        <v>214</v>
       </c>
       <c r="BA6">
-        <v>2076</v>
+        <v>4113</v>
       </c>
       <c r="BB6" t="b">
         <v>1</v>
@@ -1529,7 +1529,7 @@
         <v>1</v>
       </c>
       <c r="P7">
-        <v>990</v>
+        <v>1962</v>
       </c>
       <c r="Q7">
         <v>50</v>
@@ -1557,48 +1557,48 @@
         <v>1.35</v>
       </c>
       <c r="Y7">
-        <v>7788</v>
+        <v>15432</v>
       </c>
       <c r="Z7">
-        <v>3894</v>
+        <v>7716</v>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>457 x 191 x 106</t>
+          <t>1016 x 305 x 222</t>
         </is>
       </c>
       <c r="AB7">
         <v>345</v>
       </c>
       <c r="AC7">
-        <v>9315</v>
+        <v>19527</v>
       </c>
       <c r="AD7">
-        <v>12512</v>
+        <v>104398</v>
       </c>
       <c r="AE7">
-        <v>0.86</v>
+        <v>0.43</v>
       </c>
       <c r="AF7">
         <v>0.21</v>
       </c>
       <c r="AG7">
-        <v>0.76</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="AH7">
-        <v>7060</v>
+        <v>18434</v>
       </c>
       <c r="AI7">
         <v>345</v>
       </c>
       <c r="AJ7">
-        <v>9315</v>
+        <v>19527</v>
       </c>
       <c r="AK7">
-        <v>675000</v>
+        <v>1415000</v>
       </c>
       <c r="AL7">
-        <v>172718</v>
+        <v>362068</v>
       </c>
       <c r="AM7">
         <v>0.23</v>
@@ -1610,40 +1610,40 @@
         <v>0.99</v>
       </c>
       <c r="AP7">
-        <v>9249</v>
+        <v>19388</v>
       </c>
       <c r="AQ7">
         <v>345</v>
       </c>
       <c r="AR7">
-        <v>4658</v>
+        <v>9764</v>
       </c>
       <c r="AS7">
-        <v>52023</v>
+        <v>197935</v>
       </c>
       <c r="AT7">
-        <v>0.3</v>
+        <v>0.22</v>
       </c>
       <c r="AU7">
         <v>0.21</v>
       </c>
       <c r="AV7">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="AW7">
-        <v>4554</v>
+        <v>9716</v>
       </c>
       <c r="AX7">
         <v>169281363</v>
       </c>
       <c r="AY7">
-        <v>172718</v>
+        <v>362068</v>
       </c>
       <c r="AZ7">
-        <v>231355</v>
+        <v>142</v>
       </c>
       <c r="BA7">
-        <v>1954</v>
+        <v>3872</v>
       </c>
       <c r="BB7" t="b">
         <v>1</v>
@@ -1698,7 +1698,7 @@
         <v>1</v>
       </c>
       <c r="P8">
-        <v>980</v>
+        <v>1724</v>
       </c>
       <c r="Q8">
         <v>50</v>
@@ -1726,48 +1726,48 @@
         <v>1.35</v>
       </c>
       <c r="Y8">
-        <v>8176</v>
+        <v>14384</v>
       </c>
       <c r="Z8">
-        <v>4088</v>
+        <v>7192</v>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>686 x 254 x 125</t>
+          <t>762 x 267 x 197</t>
         </is>
       </c>
       <c r="AB8">
         <v>345</v>
       </c>
       <c r="AC8">
-        <v>10971</v>
+        <v>17319</v>
       </c>
       <c r="AD8">
-        <v>15652</v>
+        <v>31835</v>
       </c>
       <c r="AE8">
-        <v>0.84</v>
+        <v>0.74</v>
       </c>
       <c r="AF8">
         <v>0.21</v>
       </c>
       <c r="AG8">
-        <v>0.77</v>
+        <v>0.83</v>
       </c>
       <c r="AH8">
-        <v>8489</v>
+        <v>14364</v>
       </c>
       <c r="AI8">
         <v>345</v>
       </c>
       <c r="AJ8">
-        <v>10971</v>
+        <v>17319</v>
       </c>
       <c r="AK8">
-        <v>795000</v>
+        <v>1255000</v>
       </c>
       <c r="AL8">
-        <v>105455</v>
+        <v>166473</v>
       </c>
       <c r="AM8">
         <v>0.32</v>
@@ -1779,19 +1779,19 @@
         <v>0.97</v>
       </c>
       <c r="AP8">
-        <v>10666</v>
+        <v>16837</v>
       </c>
       <c r="AQ8">
         <v>345</v>
       </c>
       <c r="AR8">
-        <v>5486</v>
+        <v>8660</v>
       </c>
       <c r="AS8">
-        <v>90781</v>
+        <v>169333</v>
       </c>
       <c r="AT8">
-        <v>0.25</v>
+        <v>0.23</v>
       </c>
       <c r="AU8">
         <v>0.21</v>
@@ -1800,19 +1800,19 @@
         <v>0.99</v>
       </c>
       <c r="AW8">
-        <v>5430</v>
+        <v>8610</v>
       </c>
       <c r="AX8">
         <v>169281363</v>
       </c>
       <c r="AY8">
-        <v>105455</v>
+        <v>166473</v>
       </c>
       <c r="AZ8">
-        <v>231355</v>
+        <v>188</v>
       </c>
       <c r="BA8">
-        <v>2055</v>
+        <v>3615</v>
       </c>
       <c r="BB8" t="b">
         <v>1</v>
@@ -1867,7 +1867,7 @@
         <v>1</v>
       </c>
       <c r="P9">
-        <v>980</v>
+        <v>1724</v>
       </c>
       <c r="Q9">
         <v>50</v>
@@ -1895,48 +1895,48 @@
         <v>1.35</v>
       </c>
       <c r="Y9">
-        <v>7708</v>
+        <v>13560</v>
       </c>
       <c r="Z9">
-        <v>3854</v>
+        <v>6780</v>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>457 x 191 x 106</t>
+          <t>610 x 305 x 179</t>
         </is>
       </c>
       <c r="AB9">
         <v>345</v>
       </c>
       <c r="AC9">
-        <v>9315</v>
+        <v>15732</v>
       </c>
       <c r="AD9">
-        <v>12512</v>
+        <v>39149</v>
       </c>
       <c r="AE9">
-        <v>0.86</v>
+        <v>0.63</v>
       </c>
       <c r="AF9">
         <v>0.21</v>
       </c>
       <c r="AG9">
-        <v>0.76</v>
+        <v>0.88</v>
       </c>
       <c r="AH9">
-        <v>7060</v>
+        <v>13792</v>
       </c>
       <c r="AI9">
         <v>345</v>
       </c>
       <c r="AJ9">
-        <v>9315</v>
+        <v>15732</v>
       </c>
       <c r="AK9">
-        <v>675000</v>
+        <v>1140000</v>
       </c>
       <c r="AL9">
-        <v>172718</v>
+        <v>291702</v>
       </c>
       <c r="AM9">
         <v>0.23</v>
@@ -1948,40 +1948,40 @@
         <v>0.99</v>
       </c>
       <c r="AP9">
-        <v>9249</v>
+        <v>15620</v>
       </c>
       <c r="AQ9">
         <v>345</v>
       </c>
       <c r="AR9">
-        <v>4658</v>
+        <v>7866</v>
       </c>
       <c r="AS9">
-        <v>52023</v>
+        <v>236278</v>
       </c>
       <c r="AT9">
-        <v>0.3</v>
+        <v>0.18</v>
       </c>
       <c r="AU9">
         <v>0.21</v>
       </c>
       <c r="AV9">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="AW9">
-        <v>4554</v>
+        <v>7896</v>
       </c>
       <c r="AX9">
         <v>169281363</v>
       </c>
       <c r="AY9">
-        <v>172718</v>
+        <v>291702</v>
       </c>
       <c r="AZ9">
-        <v>231355</v>
+        <v>125</v>
       </c>
       <c r="BA9">
-        <v>1934</v>
+        <v>3402</v>
       </c>
       <c r="BB9" t="b">
         <v>1</v>
@@ -2036,7 +2036,7 @@
         <v>1</v>
       </c>
       <c r="P10">
-        <v>1170</v>
+        <v>960</v>
       </c>
       <c r="Q10">
         <v>50</v>
@@ -2064,48 +2064,48 @@
         <v>1.35</v>
       </c>
       <c r="Y10">
-        <v>9762</v>
+        <v>8010</v>
       </c>
       <c r="Z10">
-        <v>4881</v>
+        <v>4005</v>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>686 x 254 x 140</t>
+          <t>686 x 254 x 125</t>
         </is>
       </c>
       <c r="AB10">
         <v>345</v>
       </c>
       <c r="AC10">
-        <v>12282</v>
+        <v>10971</v>
       </c>
       <c r="AD10">
-        <v>18040</v>
+        <v>15652</v>
       </c>
       <c r="AE10">
-        <v>0.83</v>
+        <v>0.84</v>
       </c>
       <c r="AF10">
         <v>0.21</v>
       </c>
       <c r="AG10">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
       <c r="AH10">
-        <v>9593</v>
+        <v>8489</v>
       </c>
       <c r="AI10">
         <v>345</v>
       </c>
       <c r="AJ10">
-        <v>12282</v>
+        <v>10971</v>
       </c>
       <c r="AK10">
-        <v>890000</v>
+        <v>795000</v>
       </c>
       <c r="AL10">
-        <v>118056</v>
+        <v>105455</v>
       </c>
       <c r="AM10">
         <v>0.32</v>
@@ -2117,19 +2117,19 @@
         <v>0.97</v>
       </c>
       <c r="AP10">
-        <v>11940</v>
+        <v>10666</v>
       </c>
       <c r="AQ10">
         <v>345</v>
       </c>
       <c r="AR10">
-        <v>6141</v>
+        <v>5486</v>
       </c>
       <c r="AS10">
-        <v>107362</v>
+        <v>90781</v>
       </c>
       <c r="AT10">
-        <v>0.24</v>
+        <v>0.25</v>
       </c>
       <c r="AU10">
         <v>0.21</v>
@@ -2138,19 +2138,19 @@
         <v>0.99</v>
       </c>
       <c r="AW10">
-        <v>6088</v>
+        <v>5430</v>
       </c>
       <c r="AX10">
         <v>169281363</v>
       </c>
       <c r="AY10">
-        <v>118056</v>
+        <v>105455</v>
       </c>
       <c r="AZ10">
-        <v>231355</v>
+        <v>104</v>
       </c>
       <c r="BA10">
-        <v>2453</v>
+        <v>2013</v>
       </c>
       <c r="BB10" t="b">
         <v>1</v>
@@ -2205,7 +2205,7 @@
         <v>1</v>
       </c>
       <c r="P11">
-        <v>1170</v>
+        <v>960</v>
       </c>
       <c r="Q11">
         <v>50</v>
@@ -2233,48 +2233,48 @@
         <v>1.35</v>
       </c>
       <c r="Y11">
-        <v>9204</v>
+        <v>7552</v>
       </c>
       <c r="Z11">
-        <v>4602</v>
+        <v>3776</v>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>610 x 229 x 125</t>
+          <t>533 x 210 x 101</t>
         </is>
       </c>
       <c r="AB11">
         <v>345</v>
       </c>
       <c r="AC11">
-        <v>10971</v>
+        <v>8901</v>
       </c>
       <c r="AD11">
-        <v>25230</v>
+        <v>15737</v>
       </c>
       <c r="AE11">
-        <v>0.66</v>
+        <v>0.75</v>
       </c>
       <c r="AF11">
         <v>0.21</v>
       </c>
       <c r="AG11">
-        <v>0.87</v>
+        <v>0.82</v>
       </c>
       <c r="AH11">
-        <v>9501</v>
+        <v>7316</v>
       </c>
       <c r="AI11">
         <v>345</v>
       </c>
       <c r="AJ11">
-        <v>10971</v>
+        <v>8901</v>
       </c>
       <c r="AK11">
-        <v>795000</v>
+        <v>645000</v>
       </c>
       <c r="AL11">
-        <v>203424</v>
+        <v>165042</v>
       </c>
       <c r="AM11">
         <v>0.23</v>
@@ -2286,40 +2286,40 @@
         <v>0.99</v>
       </c>
       <c r="AP11">
-        <v>10893</v>
+        <v>8838</v>
       </c>
       <c r="AQ11">
         <v>345</v>
       </c>
       <c r="AR11">
-        <v>5486</v>
+        <v>4450</v>
       </c>
       <c r="AS11">
-        <v>81454</v>
+        <v>55753</v>
       </c>
       <c r="AT11">
-        <v>0.26</v>
+        <v>0.28</v>
       </c>
       <c r="AU11">
         <v>0.21</v>
       </c>
       <c r="AV11">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="AW11">
-        <v>5413</v>
+        <v>4368</v>
       </c>
       <c r="AX11">
         <v>169281363</v>
       </c>
       <c r="AY11">
-        <v>203424</v>
+        <v>165042</v>
       </c>
       <c r="AZ11">
-        <v>231355</v>
+        <v>70</v>
       </c>
       <c r="BA11">
-        <v>2309</v>
+        <v>1895</v>
       </c>
       <c r="BB11" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
changed P inputs & corrected Med output
</commit_message>
<xml_diff>
--- a/tables/input/output_processed_table.xlsx
+++ b/tables/input/output_processed_table.xlsx
@@ -632,14 +632,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>A-L1-S1</t>
+          <t>L1-S1</t>
         </is>
       </c>
       <c r="B2">
         <v>12.5</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D2">
         <v>6</v>
@@ -726,19 +726,19 @@
         <v>4899</v>
       </c>
       <c r="AD2">
-        <v>2481</v>
+        <v>3876</v>
       </c>
       <c r="AE2">
-        <v>1.41</v>
+        <v>1.12</v>
       </c>
       <c r="AF2">
         <v>0.21</v>
       </c>
       <c r="AG2">
-        <v>0.42</v>
+        <v>0.58</v>
       </c>
       <c r="AH2">
-        <v>2035</v>
+        <v>2839</v>
       </c>
       <c r="AI2">
         <v>355</v>
@@ -750,19 +750,19 @@
         <v>345000</v>
       </c>
       <c r="AL2">
-        <v>45763</v>
+        <v>71505</v>
       </c>
       <c r="AM2">
-        <v>0.33</v>
+        <v>0.26</v>
       </c>
       <c r="AN2">
         <v>0.21</v>
       </c>
       <c r="AO2">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
       <c r="AP2">
-        <v>4757</v>
+        <v>4832</v>
       </c>
       <c r="AQ2">
         <v>355</v>
@@ -771,28 +771,28 @@
         <v>2450</v>
       </c>
       <c r="AS2">
-        <v>21141</v>
+        <v>33032</v>
       </c>
       <c r="AT2">
-        <v>0.34</v>
+        <v>0.27</v>
       </c>
       <c r="AU2">
         <v>0.21</v>
       </c>
       <c r="AV2">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="AW2">
-        <v>2371</v>
+        <v>2410</v>
       </c>
       <c r="AX2">
         <v>169281363</v>
       </c>
       <c r="AY2">
-        <v>45763</v>
+        <v>71505</v>
       </c>
       <c r="AZ2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BA2">
         <v>806</v>
@@ -804,17 +804,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A-L1-S2</t>
+          <t>L1-S2</t>
         </is>
       </c>
       <c r="B3">
         <v>9</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>9</v>
@@ -878,96 +878,96 @@
         <v>1.35</v>
       </c>
       <c r="X3">
-        <v>286</v>
+        <v>219</v>
       </c>
       <c r="Y3">
-        <v>2984</v>
+        <v>2242</v>
       </c>
       <c r="Z3">
-        <v>1492</v>
+        <v>1121</v>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>356 x 171 x 45</t>
+          <t>305 x 127 x 37</t>
         </is>
       </c>
       <c r="AB3">
         <v>355</v>
       </c>
       <c r="AC3">
-        <v>4068</v>
+        <v>3351</v>
       </c>
       <c r="AD3">
-        <v>3096</v>
+        <v>2867</v>
       </c>
       <c r="AE3">
-        <v>1.15</v>
+        <v>1.08</v>
       </c>
       <c r="AF3">
         <v>0.21</v>
       </c>
       <c r="AG3">
-        <v>0.5600000000000001</v>
+        <v>0.61</v>
       </c>
       <c r="AH3">
-        <v>2298</v>
+        <v>2041</v>
       </c>
       <c r="AI3">
         <v>355</v>
       </c>
       <c r="AJ3">
-        <v>4068</v>
+        <v>3351</v>
       </c>
       <c r="AK3">
-        <v>286500</v>
+        <v>236000</v>
       </c>
       <c r="AL3">
-        <v>73309</v>
+        <v>94355</v>
       </c>
       <c r="AM3">
-        <v>0.24</v>
+        <v>0.19</v>
       </c>
       <c r="AN3">
         <v>0.21</v>
       </c>
       <c r="AO3">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="AP3">
-        <v>4036</v>
+        <v>3360</v>
       </c>
       <c r="AQ3">
         <v>355</v>
       </c>
       <c r="AR3">
-        <v>2034</v>
+        <v>1676</v>
       </c>
       <c r="AS3">
-        <v>16809</v>
+        <v>10881</v>
       </c>
       <c r="AT3">
-        <v>0.35</v>
+        <v>0.39</v>
       </c>
       <c r="AU3">
         <v>0.21</v>
       </c>
       <c r="AV3">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="AW3">
-        <v>1965</v>
+        <v>1600</v>
       </c>
       <c r="AX3">
         <v>169281363</v>
       </c>
       <c r="AY3">
-        <v>73309</v>
+        <v>94355</v>
       </c>
       <c r="AZ3">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="BA3">
-        <v>749</v>
+        <v>563</v>
       </c>
       <c r="BB3" t="b">
         <v>1</v>
@@ -976,14 +976,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>A-L2-S1</t>
+          <t>L2-S1</t>
         </is>
       </c>
       <c r="B4">
         <v>12.5</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -1067,19 +1067,19 @@
         <v>12282</v>
       </c>
       <c r="AD4">
-        <v>18040</v>
+        <v>28188</v>
       </c>
       <c r="AE4">
-        <v>0.83</v>
+        <v>0.66</v>
       </c>
       <c r="AF4">
         <v>0.21</v>
       </c>
       <c r="AG4">
-        <v>0.78</v>
+        <v>0.87</v>
       </c>
       <c r="AH4">
-        <v>9593</v>
+        <v>10632</v>
       </c>
       <c r="AI4">
         <v>345</v>
@@ -1091,19 +1091,19 @@
         <v>890000</v>
       </c>
       <c r="AL4">
-        <v>118056</v>
+        <v>184463</v>
       </c>
       <c r="AM4">
-        <v>0.32</v>
+        <v>0.26</v>
       </c>
       <c r="AN4">
         <v>0.21</v>
       </c>
       <c r="AO4">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
       <c r="AP4">
-        <v>11940</v>
+        <v>12124</v>
       </c>
       <c r="AQ4">
         <v>345</v>
@@ -1112,31 +1112,31 @@
         <v>6141</v>
       </c>
       <c r="AS4">
-        <v>107362</v>
+        <v>167752</v>
       </c>
       <c r="AT4">
-        <v>0.24</v>
+        <v>0.19</v>
       </c>
       <c r="AU4">
         <v>0.21</v>
       </c>
       <c r="AV4">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="AW4">
-        <v>6088</v>
+        <v>6153</v>
       </c>
       <c r="AX4">
         <v>169281363</v>
       </c>
       <c r="AY4">
-        <v>118056</v>
+        <v>184463</v>
       </c>
       <c r="AZ4">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="BA4">
-        <v>2441</v>
+        <v>2440</v>
       </c>
       <c r="BB4" t="b">
         <v>1</v>
@@ -1145,17 +1145,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>A-L2-S2</t>
+          <t>L2-S2</t>
         </is>
       </c>
       <c r="B5">
         <v>9</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>9</v>
@@ -1219,72 +1219,72 @@
         <v>1.35</v>
       </c>
       <c r="Y5">
-        <v>9156</v>
+        <v>6866</v>
       </c>
       <c r="Z5">
-        <v>4578</v>
+        <v>3433</v>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>610 x 229 x 125</t>
+          <t>533 x 210 x 92</t>
         </is>
       </c>
       <c r="AB5">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="AC5">
-        <v>10971</v>
+        <v>8307</v>
       </c>
       <c r="AD5">
-        <v>25230</v>
+        <v>22070</v>
       </c>
       <c r="AE5">
-        <v>0.66</v>
+        <v>0.61</v>
       </c>
       <c r="AF5">
         <v>0.21</v>
       </c>
       <c r="AG5">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
       <c r="AH5">
-        <v>9501</v>
+        <v>7350</v>
       </c>
       <c r="AI5">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="AJ5">
-        <v>10971</v>
+        <v>8307</v>
       </c>
       <c r="AK5">
-        <v>795000</v>
+        <v>585000</v>
       </c>
       <c r="AL5">
-        <v>203424</v>
+        <v>233889</v>
       </c>
       <c r="AM5">
+        <v>0.19</v>
+      </c>
+      <c r="AN5">
+        <v>0.21</v>
+      </c>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
+        <v>8328</v>
+      </c>
+      <c r="AQ5">
+        <v>355</v>
+      </c>
+      <c r="AR5">
+        <v>4154</v>
+      </c>
+      <c r="AS5">
+        <v>77399</v>
+      </c>
+      <c r="AT5">
         <v>0.23</v>
-      </c>
-      <c r="AN5">
-        <v>0.21</v>
-      </c>
-      <c r="AO5">
-        <v>0.99</v>
-      </c>
-      <c r="AP5">
-        <v>10893</v>
-      </c>
-      <c r="AQ5">
-        <v>345</v>
-      </c>
-      <c r="AR5">
-        <v>5486</v>
-      </c>
-      <c r="AS5">
-        <v>81454</v>
-      </c>
-      <c r="AT5">
-        <v>0.26</v>
       </c>
       <c r="AU5">
         <v>0.21</v>
@@ -1293,19 +1293,19 @@
         <v>0.99</v>
       </c>
       <c r="AW5">
-        <v>5413</v>
+        <v>4125</v>
       </c>
       <c r="AX5">
         <v>169281363</v>
       </c>
       <c r="AY5">
-        <v>203424</v>
+        <v>233889</v>
       </c>
       <c r="AZ5">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="BA5">
-        <v>2297</v>
+        <v>1723</v>
       </c>
       <c r="BB5" t="b">
         <v>1</v>
@@ -1314,14 +1314,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>A-L3-S1</t>
+          <t>L3-S1</t>
         </is>
       </c>
       <c r="B6">
         <v>12.5</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D6">
         <v>6</v>
@@ -1405,19 +1405,19 @@
         <v>19734</v>
       </c>
       <c r="AD6">
-        <v>49875</v>
+        <v>77930</v>
       </c>
       <c r="AE6">
-        <v>0.63</v>
+        <v>0.5</v>
       </c>
       <c r="AF6">
         <v>0.21</v>
       </c>
       <c r="AG6">
-        <v>0.88</v>
+        <v>0.92</v>
       </c>
       <c r="AH6">
-        <v>17339</v>
+        <v>18220</v>
       </c>
       <c r="AI6">
         <v>345</v>
@@ -1429,19 +1429,19 @@
         <v>1430000</v>
       </c>
       <c r="AL6">
-        <v>189686</v>
+        <v>296384</v>
       </c>
       <c r="AM6">
-        <v>0.32</v>
+        <v>0.26</v>
       </c>
       <c r="AN6">
         <v>0.21</v>
       </c>
       <c r="AO6">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
       <c r="AP6">
-        <v>19185</v>
+        <v>19480</v>
       </c>
       <c r="AQ6">
         <v>345</v>
@@ -1450,28 +1450,28 @@
         <v>9867</v>
       </c>
       <c r="AS6">
-        <v>232133</v>
+        <v>362708</v>
       </c>
       <c r="AT6">
-        <v>0.21</v>
+        <v>0.16</v>
       </c>
       <c r="AU6">
         <v>0.21</v>
       </c>
       <c r="AV6">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="AW6">
-        <v>9854</v>
+        <v>9942</v>
       </c>
       <c r="AX6">
         <v>169281363</v>
       </c>
       <c r="AY6">
-        <v>189686</v>
+        <v>296384</v>
       </c>
       <c r="AZ6">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="BA6">
         <v>4113</v>
@@ -1483,17 +1483,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>A-L3-S2</t>
+          <t>L3-S2</t>
         </is>
       </c>
       <c r="B7">
         <v>9</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <v>9</v>
@@ -1557,72 +1557,72 @@
         <v>1.35</v>
       </c>
       <c r="Y7">
-        <v>15432</v>
+        <v>11574</v>
       </c>
       <c r="Z7">
-        <v>7716</v>
+        <v>5787</v>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>1016 x 305 x 222</t>
+          <t>686 x 254 x 152</t>
         </is>
       </c>
       <c r="AB7">
         <v>345</v>
       </c>
       <c r="AC7">
-        <v>19527</v>
+        <v>13386</v>
       </c>
       <c r="AD7">
-        <v>104398</v>
+        <v>59972</v>
       </c>
       <c r="AE7">
-        <v>0.43</v>
+        <v>0.47</v>
       </c>
       <c r="AF7">
         <v>0.21</v>
       </c>
       <c r="AG7">
-        <v>0.9399999999999999</v>
+        <v>0.93</v>
       </c>
       <c r="AH7">
-        <v>18434</v>
+        <v>12484</v>
       </c>
       <c r="AI7">
         <v>345</v>
       </c>
       <c r="AJ7">
-        <v>19527</v>
+        <v>13386</v>
       </c>
       <c r="AK7">
-        <v>1415000</v>
+        <v>970000</v>
       </c>
       <c r="AL7">
-        <v>362068</v>
+        <v>387816</v>
       </c>
       <c r="AM7">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="AN7">
         <v>0.21</v>
       </c>
       <c r="AO7">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="AP7">
-        <v>19388</v>
+        <v>13428</v>
       </c>
       <c r="AQ7">
         <v>345</v>
       </c>
       <c r="AR7">
-        <v>9764</v>
+        <v>6693</v>
       </c>
       <c r="AS7">
-        <v>197935</v>
+        <v>187183</v>
       </c>
       <c r="AT7">
-        <v>0.22</v>
+        <v>0.19</v>
       </c>
       <c r="AU7">
         <v>0.21</v>
@@ -1631,19 +1631,19 @@
         <v>1</v>
       </c>
       <c r="AW7">
-        <v>9716</v>
+        <v>6709</v>
       </c>
       <c r="AX7">
         <v>169281363</v>
       </c>
       <c r="AY7">
-        <v>362068</v>
+        <v>387816</v>
       </c>
       <c r="AZ7">
-        <v>142</v>
+        <v>106</v>
       </c>
       <c r="BA7">
-        <v>3872</v>
+        <v>2904</v>
       </c>
       <c r="BB7" t="b">
         <v>1</v>
@@ -1652,14 +1652,14 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>A-L3-S1</t>
+          <t>L4-S1</t>
         </is>
       </c>
       <c r="B8">
         <v>12.5</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -1743,19 +1743,19 @@
         <v>17319</v>
       </c>
       <c r="AD8">
-        <v>31835</v>
+        <v>49743</v>
       </c>
       <c r="AE8">
-        <v>0.74</v>
+        <v>0.59</v>
       </c>
       <c r="AF8">
         <v>0.21</v>
       </c>
       <c r="AG8">
-        <v>0.83</v>
+        <v>0.89</v>
       </c>
       <c r="AH8">
-        <v>14364</v>
+        <v>15478</v>
       </c>
       <c r="AI8">
         <v>345</v>
@@ -1767,19 +1767,19 @@
         <v>1255000</v>
       </c>
       <c r="AL8">
-        <v>166473</v>
+        <v>260113</v>
       </c>
       <c r="AM8">
-        <v>0.32</v>
+        <v>0.26</v>
       </c>
       <c r="AN8">
         <v>0.21</v>
       </c>
       <c r="AO8">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
       <c r="AP8">
-        <v>16837</v>
+        <v>17096</v>
       </c>
       <c r="AQ8">
         <v>345</v>
@@ -1788,31 +1788,31 @@
         <v>8660</v>
       </c>
       <c r="AS8">
-        <v>169333</v>
+        <v>264583</v>
       </c>
       <c r="AT8">
-        <v>0.23</v>
+        <v>0.18</v>
       </c>
       <c r="AU8">
         <v>0.21</v>
       </c>
       <c r="AV8">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="AW8">
-        <v>8610</v>
+        <v>8696</v>
       </c>
       <c r="AX8">
         <v>169281363</v>
       </c>
       <c r="AY8">
-        <v>166473</v>
+        <v>260113</v>
       </c>
       <c r="AZ8">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="BA8">
-        <v>3615</v>
+        <v>3614</v>
       </c>
       <c r="BB8" t="b">
         <v>1</v>
@@ -1821,17 +1821,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>A-L3-S2</t>
+          <t>L4-S2</t>
         </is>
       </c>
       <c r="B9">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>9</v>
@@ -1895,72 +1895,72 @@
         <v>1.35</v>
       </c>
       <c r="Y9">
-        <v>13560</v>
+        <v>10170</v>
       </c>
       <c r="Z9">
-        <v>6780</v>
+        <v>5085</v>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>610 x 305 x 179</t>
+          <t>686 x 254 x 140</t>
         </is>
       </c>
       <c r="AB9">
         <v>345</v>
       </c>
       <c r="AC9">
-        <v>15732</v>
+        <v>12282</v>
       </c>
       <c r="AD9">
-        <v>39149</v>
+        <v>54374</v>
       </c>
       <c r="AE9">
-        <v>0.63</v>
+        <v>0.48</v>
       </c>
       <c r="AF9">
         <v>0.21</v>
       </c>
       <c r="AG9">
-        <v>0.88</v>
+        <v>0.93</v>
       </c>
       <c r="AH9">
-        <v>13792</v>
+        <v>11444</v>
       </c>
       <c r="AI9">
         <v>345</v>
       </c>
       <c r="AJ9">
-        <v>15732</v>
+        <v>12282</v>
       </c>
       <c r="AK9">
-        <v>1140000</v>
+        <v>890000</v>
       </c>
       <c r="AL9">
-        <v>291702</v>
+        <v>355831</v>
       </c>
       <c r="AM9">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="AN9">
         <v>0.21</v>
       </c>
       <c r="AO9">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="AP9">
-        <v>15620</v>
+        <v>12320</v>
       </c>
       <c r="AQ9">
         <v>345</v>
       </c>
       <c r="AR9">
-        <v>7866</v>
+        <v>6141</v>
       </c>
       <c r="AS9">
-        <v>236278</v>
+        <v>167752</v>
       </c>
       <c r="AT9">
-        <v>0.18</v>
+        <v>0.19</v>
       </c>
       <c r="AU9">
         <v>0.21</v>
@@ -1969,19 +1969,19 @@
         <v>1</v>
       </c>
       <c r="AW9">
-        <v>7896</v>
+        <v>6153</v>
       </c>
       <c r="AX9">
         <v>169281363</v>
       </c>
       <c r="AY9">
-        <v>291702</v>
+        <v>355831</v>
       </c>
       <c r="AZ9">
-        <v>125</v>
+        <v>93</v>
       </c>
       <c r="BA9">
-        <v>3402</v>
+        <v>2552</v>
       </c>
       <c r="BB9" t="b">
         <v>1</v>
@@ -1990,14 +1990,14 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>A-L3-S1</t>
+          <t>L5-S1</t>
         </is>
       </c>
       <c r="B10">
         <v>12.5</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -2081,19 +2081,19 @@
         <v>10971</v>
       </c>
       <c r="AD10">
-        <v>15652</v>
+        <v>24457</v>
       </c>
       <c r="AE10">
-        <v>0.84</v>
+        <v>0.67</v>
       </c>
       <c r="AF10">
         <v>0.21</v>
       </c>
       <c r="AG10">
-        <v>0.77</v>
+        <v>0.86</v>
       </c>
       <c r="AH10">
-        <v>8489</v>
+        <v>9451</v>
       </c>
       <c r="AI10">
         <v>345</v>
@@ -2105,19 +2105,19 @@
         <v>795000</v>
       </c>
       <c r="AL10">
-        <v>105455</v>
+        <v>164773</v>
       </c>
       <c r="AM10">
-        <v>0.32</v>
+        <v>0.26</v>
       </c>
       <c r="AN10">
         <v>0.21</v>
       </c>
       <c r="AO10">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
       <c r="AP10">
-        <v>10666</v>
+        <v>10830</v>
       </c>
       <c r="AQ10">
         <v>345</v>
@@ -2126,28 +2126,28 @@
         <v>5486</v>
       </c>
       <c r="AS10">
-        <v>90781</v>
+        <v>141845</v>
       </c>
       <c r="AT10">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="AU10">
         <v>0.21</v>
       </c>
       <c r="AV10">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="AW10">
-        <v>5430</v>
+        <v>5490</v>
       </c>
       <c r="AX10">
         <v>169281363</v>
       </c>
       <c r="AY10">
-        <v>105455</v>
+        <v>164773</v>
       </c>
       <c r="AZ10">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="BA10">
         <v>2013</v>
@@ -2159,17 +2159,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>A-L3-S2</t>
+          <t>L5-S2</t>
         </is>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>9</v>
@@ -2233,93 +2233,93 @@
         <v>1.35</v>
       </c>
       <c r="Y11">
-        <v>7552</v>
+        <v>5664</v>
       </c>
       <c r="Z11">
-        <v>3776</v>
+        <v>2832</v>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>533 x 210 x 101</t>
+          <t>406 x 178 x 74</t>
         </is>
       </c>
       <c r="AB11">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="AC11">
-        <v>8901</v>
+        <v>6710</v>
       </c>
       <c r="AD11">
-        <v>15737</v>
+        <v>10915</v>
       </c>
       <c r="AE11">
-        <v>0.75</v>
+        <v>0.78</v>
       </c>
       <c r="AF11">
         <v>0.21</v>
       </c>
       <c r="AG11">
-        <v>0.82</v>
+        <v>0.8</v>
       </c>
       <c r="AH11">
-        <v>7316</v>
+        <v>5399</v>
       </c>
       <c r="AI11">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="AJ11">
-        <v>8901</v>
+        <v>6710</v>
       </c>
       <c r="AK11">
-        <v>645000</v>
+        <v>472500</v>
       </c>
       <c r="AL11">
-        <v>165042</v>
+        <v>188910</v>
       </c>
       <c r="AM11">
-        <v>0.23</v>
+        <v>0.19</v>
       </c>
       <c r="AN11">
         <v>0.21</v>
       </c>
       <c r="AO11">
+        <v>1</v>
+      </c>
+      <c r="AP11">
+        <v>6726</v>
+      </c>
+      <c r="AQ11">
+        <v>355</v>
+      </c>
+      <c r="AR11">
+        <v>3355</v>
+      </c>
+      <c r="AS11">
+        <v>50196</v>
+      </c>
+      <c r="AT11">
+        <v>0.26</v>
+      </c>
+      <c r="AU11">
+        <v>0.21</v>
+      </c>
+      <c r="AV11">
         <v>0.99</v>
       </c>
-      <c r="AP11">
-        <v>8838</v>
-      </c>
-      <c r="AQ11">
-        <v>345</v>
-      </c>
-      <c r="AR11">
-        <v>4450</v>
-      </c>
-      <c r="AS11">
-        <v>55753</v>
-      </c>
-      <c r="AT11">
-        <v>0.28</v>
-      </c>
-      <c r="AU11">
-        <v>0.21</v>
-      </c>
-      <c r="AV11">
-        <v>0.98</v>
-      </c>
       <c r="AW11">
-        <v>4368</v>
+        <v>3311</v>
       </c>
       <c r="AX11">
         <v>169281363</v>
       </c>
       <c r="AY11">
-        <v>165042</v>
+        <v>188910</v>
       </c>
       <c r="AZ11">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="BA11">
-        <v>1895</v>
+        <v>1421</v>
       </c>
       <c r="BB11" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
major bug fixes - STABLE version
</commit_message>
<xml_diff>
--- a/tables/input/output_processed_table.xlsx
+++ b/tables/input/output_processed_table.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB11"/>
+  <dimension ref="A1:BE11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -435,7 +435,7 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>P.kN.m</t>
+          <t>Ned_no_TL.kN</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
@@ -480,127 +480,127 @@
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>Ned_2</t>
+          <t>Ned</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>Ned</t>
+          <t>selected_member_size</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>selected_member_size</t>
+          <t>fy_1</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>fy_1</t>
+          <t>N_pl_Rd_1</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>N_pl_Rd_1</t>
+          <t>Ncr_1</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>Ncr_1</t>
+          <t>lambda_bar_1</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>lambda_bar_1</t>
+          <t>alpha_yy_1</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>alpha_yy_1</t>
+          <t>X_1</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>X_1</t>
+          <t>N_b_Rd_X</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>N_b_Rd_X</t>
+          <t>fy_2</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>fy_2</t>
+          <t>N_pl_Rd_2</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>N_pl_Rd_2</t>
+          <t>Ieff_2</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>Ieff_2</t>
+          <t>Ncr_2</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
         <is>
-          <t>Ncr_2</t>
+          <t>lambda_bar_2</t>
         </is>
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>lambda_bar_2</t>
+          <t>alpha_yy_2</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
         <is>
-          <t>alpha_yy_2</t>
+          <t>X_2</t>
         </is>
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>X_2</t>
+          <t>N_b_Rd_Y</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
         <is>
-          <t>N_b_Rd_Y</t>
+          <t>fy_3</t>
         </is>
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>fy_3</t>
+          <t>N_pl_Rd_3</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
-          <t>N_pl_Rd_3</t>
+          <t>Ncr_3</t>
         </is>
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>Ncr_3</t>
+          <t>lambda_bar_3</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
-          <t>lambda_bar_3</t>
+          <t>alpha_yy_3</t>
         </is>
       </c>
       <c r="AU1" s="1" t="inlineStr">
         <is>
-          <t>alpha_yy_3</t>
+          <t>X_3</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
         <is>
-          <t>X_3</t>
+          <t>N_b_Rd_ch</t>
         </is>
       </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
-          <t>N_b_Rd_ch</t>
+          <t>DL</t>
         </is>
       </c>
       <c r="AX1" s="1" t="inlineStr">
@@ -615,15 +615,30 @@
       </c>
       <c r="AZ1" s="1" t="inlineStr">
         <is>
-          <t>MEd</t>
+          <t>load</t>
         </is>
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
+          <t>Ved</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>MEd_1st</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>MEd_2nd</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
           <t>N_ch_Ed</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
         <is>
           <t>final_check</t>
         </is>
@@ -648,7 +663,7 @@
         <v>12.5</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="G2">
         <v>90</v>
@@ -663,7 +678,7 @@
         <v>2</v>
       </c>
       <c r="K2">
-        <v>1140</v>
+        <v>1510</v>
       </c>
       <c r="L2">
         <v>210</v>
@@ -678,7 +693,7 @@
         <v>1</v>
       </c>
       <c r="P2">
-        <v>686</v>
+        <v>4122</v>
       </c>
       <c r="Q2">
         <v>50</v>
@@ -705,99 +720,112 @@
       <c r="W2">
         <v>1.35</v>
       </c>
-      <c r="X2">
-        <v>345</v>
-      </c>
-      <c r="Y2">
-        <v>3208</v>
-      </c>
-      <c r="Z2">
-        <v>1604</v>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>406 x 178 x 54</t>
-        </is>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>231</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>4353</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>406 x 178 x 60</t>
+        </is>
+      </c>
+      <c r="AA2">
+        <v>355</v>
       </c>
       <c r="AB2">
+        <v>5432</v>
+      </c>
+      <c r="AC2">
+        <v>4477</v>
+      </c>
+      <c r="AD2">
+        <v>1.1</v>
+      </c>
+      <c r="AE2">
+        <v>0.21</v>
+      </c>
+      <c r="AF2">
+        <v>0.6</v>
+      </c>
+      <c r="AG2">
+        <v>3232</v>
+      </c>
+      <c r="AH2">
         <v>355</v>
       </c>
-      <c r="AC2">
-        <v>4899</v>
-      </c>
-      <c r="AD2">
-        <v>3876</v>
-      </c>
-      <c r="AE2">
-        <v>1.12</v>
-      </c>
-      <c r="AF2">
-        <v>0.21</v>
-      </c>
-      <c r="AG2">
-        <v>0.58</v>
-      </c>
-      <c r="AH2">
-        <v>2839</v>
-      </c>
       <c r="AI2">
+        <v>5432</v>
+      </c>
+      <c r="AJ2">
+        <v>382500</v>
+      </c>
+      <c r="AK2">
+        <v>79278</v>
+      </c>
+      <c r="AL2">
+        <v>0.26</v>
+      </c>
+      <c r="AM2">
+        <v>0.21</v>
+      </c>
+      <c r="AN2">
+        <v>0.99</v>
+      </c>
+      <c r="AO2">
+        <v>5357</v>
+      </c>
+      <c r="AP2">
         <v>355</v>
       </c>
-      <c r="AJ2">
-        <v>4899</v>
-      </c>
-      <c r="AK2">
-        <v>345000</v>
-      </c>
-      <c r="AL2">
-        <v>71505</v>
-      </c>
-      <c r="AM2">
+      <c r="AQ2">
+        <v>2716</v>
+      </c>
+      <c r="AR2">
+        <v>38862</v>
+      </c>
+      <c r="AS2">
         <v>0.26</v>
       </c>
-      <c r="AN2">
-        <v>0.21</v>
-      </c>
-      <c r="AO2">
+      <c r="AT2">
+        <v>0.21</v>
+      </c>
+      <c r="AU2">
         <v>0.99</v>
       </c>
-      <c r="AP2">
-        <v>4832</v>
-      </c>
-      <c r="AQ2">
-        <v>355</v>
-      </c>
-      <c r="AR2">
-        <v>2450</v>
-      </c>
-      <c r="AS2">
-        <v>33032</v>
-      </c>
-      <c r="AT2">
-        <v>0.27</v>
-      </c>
-      <c r="AU2">
-        <v>0.21</v>
-      </c>
       <c r="AV2">
-        <v>0.98</v>
+        <v>2677</v>
       </c>
       <c r="AW2">
-        <v>2410</v>
+        <v>0.59</v>
       </c>
       <c r="AX2">
-        <v>169281363</v>
+        <v>224223560</v>
       </c>
       <c r="AY2">
-        <v>71505</v>
+        <v>79278</v>
       </c>
       <c r="AZ2">
-        <v>41</v>
+        <v>348</v>
       </c>
       <c r="BA2">
-        <v>806</v>
-      </c>
-      <c r="BB2" t="b">
+        <v>2610</v>
+      </c>
+      <c r="BB2">
+        <v>4360</v>
+      </c>
+      <c r="BC2">
+        <v>4741</v>
+      </c>
+      <c r="BD2">
+        <v>2651</v>
+      </c>
+      <c r="BE2" t="b">
         <v>1</v>
       </c>
     </row>
@@ -808,19 +836,19 @@
         </is>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>0.8</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G3">
         <v>45</v>
@@ -835,7 +863,7 @@
         <v>2</v>
       </c>
       <c r="K3">
-        <v>1140</v>
+        <v>1510</v>
       </c>
       <c r="L3">
         <v>210</v>
@@ -850,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="P3">
-        <v>686</v>
+        <v>4122</v>
       </c>
       <c r="Q3">
         <v>50</v>
@@ -877,99 +905,112 @@
       <c r="W3">
         <v>1.35</v>
       </c>
-      <c r="X3">
-        <v>219</v>
-      </c>
-      <c r="Y3">
-        <v>2242</v>
-      </c>
-      <c r="Z3">
-        <v>1121</v>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>305 x 127 x 37</t>
-        </is>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>201</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>4323</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>457 x 152 x 52</t>
+        </is>
+      </c>
+      <c r="AA3">
+        <v>355</v>
       </c>
       <c r="AB3">
+        <v>4729</v>
+      </c>
+      <c r="AC3">
+        <v>14143</v>
+      </c>
+      <c r="AD3">
+        <v>0.58</v>
+      </c>
+      <c r="AE3">
+        <v>0.21</v>
+      </c>
+      <c r="AF3">
+        <v>0.9</v>
+      </c>
+      <c r="AG3">
+        <v>4247</v>
+      </c>
+      <c r="AH3">
         <v>355</v>
       </c>
-      <c r="AC3">
-        <v>3351</v>
-      </c>
-      <c r="AD3">
-        <v>2867</v>
-      </c>
-      <c r="AE3">
-        <v>1.08</v>
-      </c>
-      <c r="AF3">
-        <v>0.21</v>
-      </c>
-      <c r="AG3">
-        <v>0.61</v>
-      </c>
-      <c r="AH3">
-        <v>2041</v>
-      </c>
       <c r="AI3">
+        <v>4729</v>
+      </c>
+      <c r="AJ3">
+        <v>333000</v>
+      </c>
+      <c r="AK3">
+        <v>220083</v>
+      </c>
+      <c r="AL3">
+        <v>0.15</v>
+      </c>
+      <c r="AM3">
+        <v>0.21</v>
+      </c>
+      <c r="AN3">
+        <v>1.01</v>
+      </c>
+      <c r="AO3">
+        <v>4783</v>
+      </c>
+      <c r="AP3">
         <v>355</v>
       </c>
-      <c r="AJ3">
-        <v>3351</v>
-      </c>
-      <c r="AK3">
-        <v>236000</v>
-      </c>
-      <c r="AL3">
-        <v>94355</v>
-      </c>
-      <c r="AM3">
-        <v>0.19</v>
-      </c>
-      <c r="AN3">
-        <v>0.21</v>
-      </c>
-      <c r="AO3">
-        <v>1</v>
-      </c>
-      <c r="AP3">
-        <v>3360</v>
-      </c>
       <c r="AQ3">
-        <v>355</v>
+        <v>2364</v>
       </c>
       <c r="AR3">
-        <v>1676</v>
+        <v>20888</v>
       </c>
       <c r="AS3">
-        <v>10881</v>
+        <v>0.34</v>
       </c>
       <c r="AT3">
-        <v>0.39</v>
+        <v>0.21</v>
       </c>
       <c r="AU3">
-        <v>0.21</v>
+        <v>0.97</v>
       </c>
       <c r="AV3">
-        <v>0.95</v>
+        <v>2291</v>
       </c>
       <c r="AW3">
-        <v>1600</v>
+        <v>0.51</v>
       </c>
       <c r="AX3">
-        <v>169281363</v>
+        <v>224223560</v>
       </c>
       <c r="AY3">
-        <v>94355</v>
+        <v>220083</v>
       </c>
       <c r="AZ3">
-        <v>20</v>
+        <v>303</v>
       </c>
       <c r="BA3">
-        <v>563</v>
-      </c>
-      <c r="BB3" t="b">
+        <v>1273</v>
+      </c>
+      <c r="BB3">
+        <v>1197</v>
+      </c>
+      <c r="BC3">
+        <v>1287</v>
+      </c>
+      <c r="BD3">
+        <v>2290</v>
+      </c>
+      <c r="BE3" t="b">
         <v>1</v>
       </c>
     </row>
@@ -992,7 +1033,7 @@
         <v>12.5</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="G4">
         <v>90</v>
@@ -1007,7 +1048,7 @@
         <v>2</v>
       </c>
       <c r="K4">
-        <v>1140</v>
+        <v>1510</v>
       </c>
       <c r="L4">
         <v>210</v>
@@ -1022,7 +1063,7 @@
         <v>1</v>
       </c>
       <c r="P4">
-        <v>1164</v>
+        <v>6987</v>
       </c>
       <c r="Q4">
         <v>50</v>
@@ -1049,96 +1090,112 @@
       <c r="W4">
         <v>1.35</v>
       </c>
-      <c r="Y4">
-        <v>9712</v>
-      </c>
-      <c r="Z4">
-        <v>4856</v>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>686 x 254 x 140</t>
-        </is>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>6987</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>610 x 178 x 82</t>
+        </is>
+      </c>
+      <c r="AA4">
+        <v>355</v>
       </c>
       <c r="AB4">
-        <v>345</v>
+        <v>7384</v>
       </c>
       <c r="AC4">
-        <v>12282</v>
+        <v>11586</v>
       </c>
       <c r="AD4">
-        <v>28188</v>
+        <v>0.8</v>
       </c>
       <c r="AE4">
-        <v>0.66</v>
+        <v>0.21</v>
       </c>
       <c r="AF4">
-        <v>0.21</v>
+        <v>0.8</v>
       </c>
       <c r="AG4">
-        <v>0.87</v>
+        <v>5883</v>
       </c>
       <c r="AH4">
-        <v>10632</v>
+        <v>355</v>
       </c>
       <c r="AI4">
-        <v>345</v>
+        <v>7384</v>
       </c>
       <c r="AJ4">
-        <v>12282</v>
+        <v>520000</v>
       </c>
       <c r="AK4">
-        <v>890000</v>
+        <v>107776</v>
       </c>
       <c r="AL4">
-        <v>184463</v>
+        <v>0.26</v>
       </c>
       <c r="AM4">
-        <v>0.26</v>
+        <v>0.21</v>
       </c>
       <c r="AN4">
-        <v>0.21</v>
+        <v>0.99</v>
       </c>
       <c r="AO4">
-        <v>0.99</v>
+        <v>7283</v>
       </c>
       <c r="AP4">
-        <v>12124</v>
+        <v>355</v>
       </c>
       <c r="AQ4">
-        <v>345</v>
+        <v>3692</v>
       </c>
       <c r="AR4">
-        <v>6141</v>
+        <v>39185</v>
       </c>
       <c r="AS4">
-        <v>167752</v>
+        <v>0.31</v>
       </c>
       <c r="AT4">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="AU4">
-        <v>0.21</v>
+        <v>0.98</v>
       </c>
       <c r="AV4">
-        <v>1</v>
+        <v>3603</v>
       </c>
       <c r="AW4">
-        <v>6153</v>
+        <v>0.8</v>
       </c>
       <c r="AX4">
-        <v>169281363</v>
+        <v>224223560</v>
       </c>
       <c r="AY4">
-        <v>184463</v>
+        <v>107776</v>
       </c>
       <c r="AZ4">
-        <v>125</v>
+        <v>51</v>
       </c>
       <c r="BA4">
-        <v>2440</v>
-      </c>
-      <c r="BB4" t="b">
+        <v>11</v>
+      </c>
+      <c r="BB4">
+        <v>640</v>
+      </c>
+      <c r="BC4">
+        <v>884</v>
+      </c>
+      <c r="BD4">
+        <v>3582</v>
+      </c>
+      <c r="BE4" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1149,19 +1206,19 @@
         </is>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>0.8</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G5">
         <v>45</v>
@@ -1176,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="K5">
-        <v>1140</v>
+        <v>1510</v>
       </c>
       <c r="L5">
         <v>210</v>
@@ -1191,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="P5">
-        <v>1164</v>
+        <v>6987</v>
       </c>
       <c r="Q5">
         <v>50</v>
@@ -1218,96 +1275,112 @@
       <c r="W5">
         <v>1.35</v>
       </c>
-      <c r="Y5">
-        <v>6866</v>
-      </c>
-      <c r="Z5">
-        <v>3433</v>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>533 x 210 x 92</t>
-        </is>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>6987</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>610 x 178 x 82</t>
+        </is>
+      </c>
+      <c r="AA5">
+        <v>355</v>
       </c>
       <c r="AB5">
+        <v>7384</v>
+      </c>
+      <c r="AC5">
+        <v>36945</v>
+      </c>
+      <c r="AD5">
+        <v>0.45</v>
+      </c>
+      <c r="AE5">
+        <v>0.21</v>
+      </c>
+      <c r="AF5">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="AG5">
+        <v>6941</v>
+      </c>
+      <c r="AH5">
         <v>355</v>
       </c>
-      <c r="AC5">
-        <v>8307</v>
-      </c>
-      <c r="AD5">
-        <v>22070</v>
-      </c>
-      <c r="AE5">
-        <v>0.61</v>
-      </c>
-      <c r="AF5">
-        <v>0.21</v>
-      </c>
-      <c r="AG5">
-        <v>0.88</v>
-      </c>
-      <c r="AH5">
-        <v>7350</v>
-      </c>
       <c r="AI5">
+        <v>7384</v>
+      </c>
+      <c r="AJ5">
+        <v>520000</v>
+      </c>
+      <c r="AK5">
+        <v>343674</v>
+      </c>
+      <c r="AL5">
+        <v>0.15</v>
+      </c>
+      <c r="AM5">
+        <v>0.21</v>
+      </c>
+      <c r="AN5">
+        <v>1.01</v>
+      </c>
+      <c r="AO5">
+        <v>7470</v>
+      </c>
+      <c r="AP5">
         <v>355</v>
       </c>
-      <c r="AJ5">
-        <v>8307</v>
-      </c>
-      <c r="AK5">
-        <v>585000</v>
-      </c>
-      <c r="AL5">
-        <v>233889</v>
-      </c>
-      <c r="AM5">
-        <v>0.19</v>
-      </c>
-      <c r="AN5">
-        <v>0.21</v>
-      </c>
-      <c r="AO5">
-        <v>1</v>
-      </c>
-      <c r="AP5">
-        <v>8328</v>
-      </c>
       <c r="AQ5">
-        <v>355</v>
+        <v>3692</v>
       </c>
       <c r="AR5">
-        <v>4154</v>
+        <v>39185</v>
       </c>
       <c r="AS5">
-        <v>77399</v>
+        <v>0.31</v>
       </c>
       <c r="AT5">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AU5">
-        <v>0.21</v>
+        <v>0.98</v>
       </c>
       <c r="AV5">
-        <v>0.99</v>
+        <v>3603</v>
       </c>
       <c r="AW5">
-        <v>4125</v>
+        <v>0.8</v>
       </c>
       <c r="AX5">
-        <v>169281363</v>
+        <v>224223560</v>
       </c>
       <c r="AY5">
-        <v>233889</v>
+        <v>343674</v>
       </c>
       <c r="AZ5">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="BA5">
-        <v>1723</v>
-      </c>
-      <c r="BB5" t="b">
+        <v>6</v>
+      </c>
+      <c r="BB5">
+        <v>202</v>
+      </c>
+      <c r="BC5">
+        <v>310</v>
+      </c>
+      <c r="BD5">
+        <v>3525</v>
+      </c>
+      <c r="BE5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1330,7 +1403,7 @@
         <v>12.5</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="G6">
         <v>90</v>
@@ -1345,7 +1418,7 @@
         <v>2</v>
       </c>
       <c r="K6">
-        <v>1140</v>
+        <v>1510</v>
       </c>
       <c r="L6">
         <v>210</v>
@@ -1360,7 +1433,7 @@
         <v>1</v>
       </c>
       <c r="P6">
-        <v>1962</v>
+        <v>11773</v>
       </c>
       <c r="Q6">
         <v>50</v>
@@ -1387,96 +1460,112 @@
       <c r="W6">
         <v>1.35</v>
       </c>
-      <c r="Y6">
-        <v>16368</v>
-      </c>
-      <c r="Z6">
-        <v>8184</v>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>914 x 305 x 224</t>
-        </is>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>11773</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>762 x 267 x 134</t>
+        </is>
+      </c>
+      <c r="AA6">
+        <v>355</v>
       </c>
       <c r="AB6">
-        <v>345</v>
+        <v>12141</v>
       </c>
       <c r="AC6">
-        <v>19734</v>
+        <v>31297</v>
       </c>
       <c r="AD6">
-        <v>77930</v>
+        <v>0.62</v>
       </c>
       <c r="AE6">
-        <v>0.5</v>
+        <v>0.21</v>
       </c>
       <c r="AF6">
-        <v>0.21</v>
+        <v>0.88</v>
       </c>
       <c r="AG6">
-        <v>0.92</v>
+        <v>10698</v>
       </c>
       <c r="AH6">
-        <v>18220</v>
+        <v>355</v>
       </c>
       <c r="AI6">
-        <v>345</v>
+        <v>12141</v>
       </c>
       <c r="AJ6">
-        <v>19734</v>
+        <v>855000</v>
       </c>
       <c r="AK6">
-        <v>1430000</v>
+        <v>177209</v>
       </c>
       <c r="AL6">
-        <v>296384</v>
+        <v>0.26</v>
       </c>
       <c r="AM6">
-        <v>0.26</v>
+        <v>0.21</v>
       </c>
       <c r="AN6">
-        <v>0.21</v>
+        <v>0.99</v>
       </c>
       <c r="AO6">
-        <v>0.99</v>
+        <v>11974</v>
       </c>
       <c r="AP6">
-        <v>19480</v>
+        <v>355</v>
       </c>
       <c r="AQ6">
-        <v>345</v>
+        <v>6070</v>
       </c>
       <c r="AR6">
-        <v>9867</v>
+        <v>155122</v>
       </c>
       <c r="AS6">
-        <v>362708</v>
+        <v>0.2</v>
       </c>
       <c r="AT6">
-        <v>0.16</v>
+        <v>0.21</v>
       </c>
       <c r="AU6">
-        <v>0.21</v>
+        <v>1</v>
       </c>
       <c r="AV6">
-        <v>1.01</v>
+        <v>6073</v>
       </c>
       <c r="AW6">
-        <v>9942</v>
+        <v>1.31</v>
       </c>
       <c r="AX6">
-        <v>169281363</v>
+        <v>224223560</v>
       </c>
       <c r="AY6">
-        <v>296384</v>
+        <v>177209</v>
       </c>
       <c r="AZ6">
-        <v>210</v>
+        <v>51</v>
       </c>
       <c r="BA6">
-        <v>4113</v>
-      </c>
-      <c r="BB6" t="b">
+        <v>11</v>
+      </c>
+      <c r="BB6">
+        <v>640</v>
+      </c>
+      <c r="BC6">
+        <v>1014</v>
+      </c>
+      <c r="BD6">
+        <v>5988</v>
+      </c>
+      <c r="BE6" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1487,19 +1576,19 @@
         </is>
       </c>
       <c r="B7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>0.8</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G7">
         <v>45</v>
@@ -1514,7 +1603,7 @@
         <v>2</v>
       </c>
       <c r="K7">
-        <v>1140</v>
+        <v>1510</v>
       </c>
       <c r="L7">
         <v>210</v>
@@ -1529,7 +1618,7 @@
         <v>1</v>
       </c>
       <c r="P7">
-        <v>1962</v>
+        <v>11773</v>
       </c>
       <c r="Q7">
         <v>50</v>
@@ -1556,96 +1645,112 @@
       <c r="W7">
         <v>1.35</v>
       </c>
-      <c r="Y7">
-        <v>11574</v>
-      </c>
-      <c r="Z7">
-        <v>5787</v>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>686 x 254 x 152</t>
-        </is>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>11773</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>762 x 267 x 134</t>
+        </is>
+      </c>
+      <c r="AA7">
+        <v>355</v>
       </c>
       <c r="AB7">
-        <v>345</v>
+        <v>12141</v>
       </c>
       <c r="AC7">
-        <v>13386</v>
+        <v>99798</v>
       </c>
       <c r="AD7">
-        <v>59972</v>
+        <v>0.35</v>
       </c>
       <c r="AE7">
-        <v>0.47</v>
+        <v>0.21</v>
       </c>
       <c r="AF7">
-        <v>0.21</v>
+        <v>0.97</v>
       </c>
       <c r="AG7">
-        <v>0.93</v>
+        <v>11726</v>
       </c>
       <c r="AH7">
-        <v>12484</v>
+        <v>355</v>
       </c>
       <c r="AI7">
-        <v>345</v>
+        <v>12141</v>
       </c>
       <c r="AJ7">
-        <v>13386</v>
+        <v>855000</v>
       </c>
       <c r="AK7">
-        <v>970000</v>
+        <v>565079</v>
       </c>
       <c r="AL7">
-        <v>387816</v>
+        <v>0.15</v>
       </c>
       <c r="AM7">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="AN7">
-        <v>0.21</v>
+        <v>1.01</v>
       </c>
       <c r="AO7">
-        <v>1</v>
+        <v>12282</v>
       </c>
       <c r="AP7">
-        <v>13428</v>
+        <v>355</v>
       </c>
       <c r="AQ7">
-        <v>345</v>
+        <v>6070</v>
       </c>
       <c r="AR7">
-        <v>6693</v>
+        <v>155122</v>
       </c>
       <c r="AS7">
-        <v>187183</v>
+        <v>0.2</v>
       </c>
       <c r="AT7">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="AU7">
-        <v>0.21</v>
+        <v>1</v>
       </c>
       <c r="AV7">
-        <v>1</v>
+        <v>6073</v>
       </c>
       <c r="AW7">
-        <v>6709</v>
+        <v>1.31</v>
       </c>
       <c r="AX7">
-        <v>169281363</v>
+        <v>224223560</v>
       </c>
       <c r="AY7">
-        <v>387816</v>
+        <v>565079</v>
       </c>
       <c r="AZ7">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="BA7">
-        <v>2904</v>
-      </c>
-      <c r="BB7" t="b">
+        <v>6</v>
+      </c>
+      <c r="BB7">
+        <v>202</v>
+      </c>
+      <c r="BC7">
+        <v>379</v>
+      </c>
+      <c r="BD7">
+        <v>5924</v>
+      </c>
+      <c r="BE7" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1668,7 +1773,7 @@
         <v>12.5</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="G8">
         <v>90</v>
@@ -1683,7 +1788,7 @@
         <v>2</v>
       </c>
       <c r="K8">
-        <v>1140</v>
+        <v>1510</v>
       </c>
       <c r="L8">
         <v>210</v>
@@ -1698,7 +1803,7 @@
         <v>1</v>
       </c>
       <c r="P8">
-        <v>1724</v>
+        <v>10347</v>
       </c>
       <c r="Q8">
         <v>50</v>
@@ -1725,96 +1830,112 @@
       <c r="W8">
         <v>1.35</v>
       </c>
-      <c r="Y8">
-        <v>14384</v>
-      </c>
-      <c r="Z8">
-        <v>7192</v>
-      </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>762 x 267 x 197</t>
-        </is>
+      <c r="X8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>10347</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>533 x 210 x 122</t>
+        </is>
+      </c>
+      <c r="AA8">
+        <v>345</v>
       </c>
       <c r="AB8">
+        <v>10695</v>
+      </c>
+      <c r="AC8">
+        <v>15752</v>
+      </c>
+      <c r="AD8">
+        <v>0.82</v>
+      </c>
+      <c r="AE8">
+        <v>0.21</v>
+      </c>
+      <c r="AF8">
+        <v>0.78</v>
+      </c>
+      <c r="AG8">
+        <v>8360</v>
+      </c>
+      <c r="AH8">
         <v>345</v>
       </c>
-      <c r="AC8">
-        <v>17319</v>
-      </c>
-      <c r="AD8">
-        <v>49743</v>
-      </c>
-      <c r="AE8">
-        <v>0.59</v>
-      </c>
-      <c r="AF8">
-        <v>0.21</v>
-      </c>
-      <c r="AG8">
-        <v>0.89</v>
-      </c>
-      <c r="AH8">
-        <v>15478</v>
-      </c>
       <c r="AI8">
+        <v>10695</v>
+      </c>
+      <c r="AJ8">
+        <v>775000</v>
+      </c>
+      <c r="AK8">
+        <v>160628</v>
+      </c>
+      <c r="AL8">
+        <v>0.26</v>
+      </c>
+      <c r="AM8">
+        <v>0.21</v>
+      </c>
+      <c r="AN8">
+        <v>0.99</v>
+      </c>
+      <c r="AO8">
+        <v>10557</v>
+      </c>
+      <c r="AP8">
         <v>345</v>
       </c>
-      <c r="AJ8">
-        <v>17319</v>
-      </c>
-      <c r="AK8">
-        <v>1255000</v>
-      </c>
-      <c r="AL8">
-        <v>260113</v>
-      </c>
-      <c r="AM8">
-        <v>0.26</v>
-      </c>
-      <c r="AN8">
-        <v>0.21</v>
-      </c>
-      <c r="AO8">
-        <v>0.99</v>
-      </c>
-      <c r="AP8">
-        <v>17096</v>
-      </c>
       <c r="AQ8">
-        <v>345</v>
+        <v>5348</v>
       </c>
       <c r="AR8">
-        <v>8660</v>
+        <v>109784</v>
       </c>
       <c r="AS8">
-        <v>264583</v>
+        <v>0.22</v>
       </c>
       <c r="AT8">
-        <v>0.18</v>
+        <v>0.21</v>
       </c>
       <c r="AU8">
-        <v>0.21</v>
+        <v>1</v>
       </c>
       <c r="AV8">
-        <v>1</v>
+        <v>5323</v>
       </c>
       <c r="AW8">
-        <v>8696</v>
+        <v>1.2</v>
       </c>
       <c r="AX8">
-        <v>169281363</v>
+        <v>224223560</v>
       </c>
       <c r="AY8">
-        <v>260113</v>
+        <v>160628</v>
       </c>
       <c r="AZ8">
-        <v>185</v>
+        <v>51</v>
       </c>
       <c r="BA8">
-        <v>3614</v>
-      </c>
-      <c r="BB8" t="b">
+        <v>11</v>
+      </c>
+      <c r="BB8">
+        <v>640</v>
+      </c>
+      <c r="BC8">
+        <v>973</v>
+      </c>
+      <c r="BD8">
+        <v>5271</v>
+      </c>
+      <c r="BE8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1825,19 +1946,19 @@
         </is>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>0.8</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E9">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G9">
         <v>45</v>
@@ -1852,7 +1973,7 @@
         <v>2</v>
       </c>
       <c r="K9">
-        <v>1140</v>
+        <v>1510</v>
       </c>
       <c r="L9">
         <v>210</v>
@@ -1867,7 +1988,7 @@
         <v>1</v>
       </c>
       <c r="P9">
-        <v>1724</v>
+        <v>10347</v>
       </c>
       <c r="Q9">
         <v>50</v>
@@ -1894,96 +2015,112 @@
       <c r="W9">
         <v>1.35</v>
       </c>
-      <c r="Y9">
-        <v>10170</v>
-      </c>
-      <c r="Z9">
-        <v>5085</v>
-      </c>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>686 x 254 x 140</t>
-        </is>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>10347</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>533 x 210 x 122</t>
+        </is>
+      </c>
+      <c r="AA9">
+        <v>345</v>
       </c>
       <c r="AB9">
+        <v>10695</v>
+      </c>
+      <c r="AC9">
+        <v>50229</v>
+      </c>
+      <c r="AD9">
+        <v>0.46</v>
+      </c>
+      <c r="AE9">
+        <v>0.21</v>
+      </c>
+      <c r="AF9">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="AG9">
+        <v>10009</v>
+      </c>
+      <c r="AH9">
         <v>345</v>
       </c>
-      <c r="AC9">
-        <v>12282</v>
-      </c>
-      <c r="AD9">
-        <v>54374</v>
-      </c>
-      <c r="AE9">
-        <v>0.48</v>
-      </c>
-      <c r="AF9">
-        <v>0.21</v>
-      </c>
-      <c r="AG9">
-        <v>0.93</v>
-      </c>
-      <c r="AH9">
-        <v>11444</v>
-      </c>
       <c r="AI9">
+        <v>10695</v>
+      </c>
+      <c r="AJ9">
+        <v>775000</v>
+      </c>
+      <c r="AK9">
+        <v>512206</v>
+      </c>
+      <c r="AL9">
+        <v>0.14</v>
+      </c>
+      <c r="AM9">
+        <v>0.21</v>
+      </c>
+      <c r="AN9">
+        <v>1.01</v>
+      </c>
+      <c r="AO9">
+        <v>10824</v>
+      </c>
+      <c r="AP9">
         <v>345</v>
       </c>
-      <c r="AJ9">
-        <v>12282</v>
-      </c>
-      <c r="AK9">
-        <v>890000</v>
-      </c>
-      <c r="AL9">
-        <v>355831</v>
-      </c>
-      <c r="AM9">
-        <v>0.19</v>
-      </c>
-      <c r="AN9">
-        <v>0.21</v>
-      </c>
-      <c r="AO9">
-        <v>1</v>
-      </c>
-      <c r="AP9">
-        <v>12320</v>
-      </c>
       <c r="AQ9">
-        <v>345</v>
+        <v>5348</v>
       </c>
       <c r="AR9">
-        <v>6141</v>
+        <v>109784</v>
       </c>
       <c r="AS9">
-        <v>167752</v>
+        <v>0.22</v>
       </c>
       <c r="AT9">
-        <v>0.19</v>
+        <v>0.21</v>
       </c>
       <c r="AU9">
-        <v>0.21</v>
+        <v>1</v>
       </c>
       <c r="AV9">
-        <v>1</v>
+        <v>5323</v>
       </c>
       <c r="AW9">
-        <v>6153</v>
+        <v>1.2</v>
       </c>
       <c r="AX9">
-        <v>169281363</v>
+        <v>224223560</v>
       </c>
       <c r="AY9">
-        <v>355831</v>
+        <v>512206</v>
       </c>
       <c r="AZ9">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="BA9">
-        <v>2552</v>
-      </c>
-      <c r="BB9" t="b">
+        <v>6</v>
+      </c>
+      <c r="BB9">
+        <v>202</v>
+      </c>
+      <c r="BC9">
+        <v>358</v>
+      </c>
+      <c r="BD9">
+        <v>5209</v>
+      </c>
+      <c r="BE9" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2006,7 +2143,7 @@
         <v>12.5</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>12.5</v>
       </c>
       <c r="G10">
         <v>90</v>
@@ -2021,7 +2158,7 @@
         <v>2</v>
       </c>
       <c r="K10">
-        <v>1140</v>
+        <v>1510</v>
       </c>
       <c r="L10">
         <v>210</v>
@@ -2036,7 +2173,7 @@
         <v>1</v>
       </c>
       <c r="P10">
-        <v>960</v>
+        <v>5765</v>
       </c>
       <c r="Q10">
         <v>50</v>
@@ -2063,96 +2200,112 @@
       <c r="W10">
         <v>1.35</v>
       </c>
-      <c r="Y10">
-        <v>8010</v>
-      </c>
-      <c r="Z10">
-        <v>4005</v>
-      </c>
-      <c r="AA10" t="inlineStr">
-        <is>
-          <t>686 x 254 x 125</t>
-        </is>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>5765</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>457 x 191 x 67</t>
+        </is>
+      </c>
+      <c r="AA10">
+        <v>355</v>
       </c>
       <c r="AB10">
-        <v>345</v>
+        <v>6070</v>
       </c>
       <c r="AC10">
-        <v>10971</v>
+        <v>6093</v>
       </c>
       <c r="AD10">
-        <v>24457</v>
+        <v>1</v>
       </c>
       <c r="AE10">
+        <v>0.21</v>
+      </c>
+      <c r="AF10">
         <v>0.67</v>
       </c>
-      <c r="AF10">
-        <v>0.21</v>
-      </c>
       <c r="AG10">
-        <v>0.86</v>
+        <v>4049</v>
       </c>
       <c r="AH10">
-        <v>9451</v>
+        <v>355</v>
       </c>
       <c r="AI10">
-        <v>345</v>
+        <v>6070</v>
       </c>
       <c r="AJ10">
-        <v>10971</v>
+        <v>427500</v>
       </c>
       <c r="AK10">
-        <v>795000</v>
+        <v>88604</v>
       </c>
       <c r="AL10">
-        <v>164773</v>
+        <v>0.26</v>
       </c>
       <c r="AM10">
-        <v>0.26</v>
+        <v>0.21</v>
       </c>
       <c r="AN10">
-        <v>0.21</v>
+        <v>0.99</v>
       </c>
       <c r="AO10">
+        <v>5987</v>
+      </c>
+      <c r="AP10">
+        <v>355</v>
+      </c>
+      <c r="AQ10">
+        <v>3035</v>
+      </c>
+      <c r="AR10">
+        <v>46958</v>
+      </c>
+      <c r="AS10">
+        <v>0.25</v>
+      </c>
+      <c r="AT10">
+        <v>0.21</v>
+      </c>
+      <c r="AU10">
         <v>0.99</v>
       </c>
-      <c r="AP10">
-        <v>10830</v>
-      </c>
-      <c r="AQ10">
-        <v>345</v>
-      </c>
-      <c r="AR10">
-        <v>5486</v>
-      </c>
-      <c r="AS10">
-        <v>141845</v>
-      </c>
-      <c r="AT10">
-        <v>0.2</v>
-      </c>
-      <c r="AU10">
-        <v>0.21</v>
-      </c>
       <c r="AV10">
-        <v>1</v>
+        <v>2999</v>
       </c>
       <c r="AW10">
-        <v>5490</v>
+        <v>0.66</v>
       </c>
       <c r="AX10">
-        <v>169281363</v>
+        <v>224223560</v>
       </c>
       <c r="AY10">
-        <v>164773</v>
+        <v>88604</v>
       </c>
       <c r="AZ10">
-        <v>103</v>
+        <v>51</v>
       </c>
       <c r="BA10">
-        <v>2013</v>
-      </c>
-      <c r="BB10" t="b">
+        <v>11</v>
+      </c>
+      <c r="BB10">
+        <v>640</v>
+      </c>
+      <c r="BC10">
+        <v>839</v>
+      </c>
+      <c r="BD10">
+        <v>2966</v>
+      </c>
+      <c r="BE10" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2163,19 +2316,19 @@
         </is>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>0.8</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E11">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G11">
         <v>45</v>
@@ -2190,7 +2343,7 @@
         <v>2</v>
       </c>
       <c r="K11">
-        <v>1140</v>
+        <v>1510</v>
       </c>
       <c r="L11">
         <v>210</v>
@@ -2205,7 +2358,7 @@
         <v>1</v>
       </c>
       <c r="P11">
-        <v>960</v>
+        <v>5765</v>
       </c>
       <c r="Q11">
         <v>50</v>
@@ -2232,96 +2385,112 @@
       <c r="W11">
         <v>1.35</v>
       </c>
-      <c r="Y11">
-        <v>5664</v>
-      </c>
-      <c r="Z11">
-        <v>2832</v>
-      </c>
-      <c r="AA11" t="inlineStr">
-        <is>
-          <t>406 x 178 x 74</t>
-        </is>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>5765</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>457 x 191 x 67</t>
+        </is>
+      </c>
+      <c r="AA11">
+        <v>355</v>
       </c>
       <c r="AB11">
+        <v>6070</v>
+      </c>
+      <c r="AC11">
+        <v>19431</v>
+      </c>
+      <c r="AD11">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="AE11">
+        <v>0.21</v>
+      </c>
+      <c r="AF11">
+        <v>0.9</v>
+      </c>
+      <c r="AG11">
+        <v>5493</v>
+      </c>
+      <c r="AH11">
         <v>355</v>
       </c>
-      <c r="AC11">
-        <v>6710</v>
-      </c>
-      <c r="AD11">
-        <v>10915</v>
-      </c>
-      <c r="AE11">
-        <v>0.78</v>
-      </c>
-      <c r="AF11">
-        <v>0.21</v>
-      </c>
-      <c r="AG11">
-        <v>0.8</v>
-      </c>
-      <c r="AH11">
-        <v>5399</v>
-      </c>
       <c r="AI11">
+        <v>6070</v>
+      </c>
+      <c r="AJ11">
+        <v>427500</v>
+      </c>
+      <c r="AK11">
+        <v>282539</v>
+      </c>
+      <c r="AL11">
+        <v>0.15</v>
+      </c>
+      <c r="AM11">
+        <v>0.21</v>
+      </c>
+      <c r="AN11">
+        <v>1.01</v>
+      </c>
+      <c r="AO11">
+        <v>6141</v>
+      </c>
+      <c r="AP11">
         <v>355</v>
       </c>
-      <c r="AJ11">
-        <v>6710</v>
-      </c>
-      <c r="AK11">
-        <v>472500</v>
-      </c>
-      <c r="AL11">
-        <v>188910</v>
-      </c>
-      <c r="AM11">
-        <v>0.19</v>
-      </c>
-      <c r="AN11">
-        <v>0.21</v>
-      </c>
-      <c r="AO11">
-        <v>1</v>
-      </c>
-      <c r="AP11">
-        <v>6726</v>
-      </c>
       <c r="AQ11">
-        <v>355</v>
+        <v>3035</v>
       </c>
       <c r="AR11">
-        <v>3355</v>
+        <v>46958</v>
       </c>
       <c r="AS11">
-        <v>50196</v>
+        <v>0.25</v>
       </c>
       <c r="AT11">
-        <v>0.26</v>
+        <v>0.21</v>
       </c>
       <c r="AU11">
-        <v>0.21</v>
+        <v>0.99</v>
       </c>
       <c r="AV11">
-        <v>0.99</v>
+        <v>2999</v>
       </c>
       <c r="AW11">
-        <v>3311</v>
+        <v>0.66</v>
       </c>
       <c r="AX11">
-        <v>169281363</v>
+        <v>224223560</v>
       </c>
       <c r="AY11">
-        <v>188910</v>
+        <v>282539</v>
       </c>
       <c r="AZ11">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="BA11">
-        <v>1421</v>
-      </c>
-      <c r="BB11" t="b">
+        <v>6</v>
+      </c>
+      <c r="BB11">
+        <v>202</v>
+      </c>
+      <c r="BC11">
+        <v>289</v>
+      </c>
+      <c r="BD11">
+        <v>2911</v>
+      </c>
+      <c r="BE11" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some calculation corrections. new STABLE version
</commit_message>
<xml_diff>
--- a/tables/input/output_processed_table.xlsx
+++ b/tables/input/output_processed_table.xlsx
@@ -656,7 +656,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>12.5</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>0.8</v>
@@ -665,10 +665,10 @@
         <v>6</v>
       </c>
       <c r="E2">
-        <v>12.5</v>
+        <v>14</v>
       </c>
       <c r="F2">
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="G2">
         <v>90</v>
@@ -750,19 +750,19 @@
         <v>3529</v>
       </c>
       <c r="AD2">
-        <v>2591</v>
+        <v>2065</v>
       </c>
       <c r="AE2">
-        <v>1.17</v>
+        <v>1.31</v>
       </c>
       <c r="AF2">
         <v>0.21</v>
       </c>
       <c r="AG2">
-        <v>0.55</v>
+        <v>0.47</v>
       </c>
       <c r="AH2">
-        <v>1945</v>
+        <v>1646</v>
       </c>
       <c r="AI2">
         <v>355</v>
@@ -774,19 +774,19 @@
         <v>248500</v>
       </c>
       <c r="AL2">
-        <v>51505</v>
+        <v>47619</v>
       </c>
       <c r="AM2">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="AN2">
         <v>0.21</v>
       </c>
       <c r="AO2">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="AP2">
-        <v>3480</v>
+        <v>3472</v>
       </c>
       <c r="AQ2">
         <v>355</v>
@@ -810,28 +810,28 @@
         <v>1697</v>
       </c>
       <c r="AX2">
-        <v>0.38</v>
+        <v>0.84</v>
       </c>
       <c r="AY2">
         <v>224223560</v>
       </c>
       <c r="AZ2">
-        <v>51505</v>
+        <v>41059</v>
       </c>
       <c r="BA2">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB2">
-        <v>382</v>
+        <v>437</v>
       </c>
       <c r="BC2">
-        <v>640</v>
+        <v>817</v>
       </c>
       <c r="BD2">
-        <v>755</v>
+        <v>966</v>
       </c>
       <c r="BE2">
-        <v>1524</v>
+        <v>1546</v>
       </c>
       <c r="BF2" t="b">
         <v>1</v>
@@ -889,7 +889,7 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q3">
-        <v>2748</v>
+        <v>1457</v>
       </c>
       <c r="R3">
         <v>50</v>
@@ -918,51 +918,51 @@
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>84</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>2890</t>
+          <t>1541</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>305 x 127 x 37</t>
+          <t>254 x 102 x 22</t>
         </is>
       </c>
       <c r="AB3">
         <v>355</v>
       </c>
       <c r="AC3">
-        <v>3351</v>
+        <v>1988</v>
       </c>
       <c r="AD3">
-        <v>4739</v>
+        <v>1877</v>
       </c>
       <c r="AE3">
-        <v>0.84</v>
+        <v>1.03</v>
       </c>
       <c r="AF3">
         <v>0.21</v>
       </c>
       <c r="AG3">
-        <v>0.77</v>
+        <v>0.65</v>
       </c>
       <c r="AH3">
-        <v>2585</v>
+        <v>1283</v>
       </c>
       <c r="AI3">
         <v>355</v>
       </c>
       <c r="AJ3">
-        <v>3351</v>
+        <v>1988</v>
       </c>
       <c r="AK3">
-        <v>236000</v>
+        <v>140000</v>
       </c>
       <c r="AL3">
-        <v>155975</v>
+        <v>92528</v>
       </c>
       <c r="AM3">
         <v>0.15</v>
@@ -974,37 +974,37 @@
         <v>1.01</v>
       </c>
       <c r="AP3">
-        <v>3390</v>
+        <v>2011</v>
       </c>
       <c r="AQ3">
         <v>355</v>
       </c>
       <c r="AR3">
-        <v>1676</v>
+        <v>994</v>
       </c>
       <c r="AS3">
-        <v>10881</v>
+        <v>3854</v>
       </c>
       <c r="AT3">
-        <v>0.39</v>
+        <v>0.51</v>
       </c>
       <c r="AU3">
         <v>0.21</v>
       </c>
       <c r="AV3">
-        <v>0.95</v>
+        <v>0.92</v>
       </c>
       <c r="AW3">
-        <v>1600</v>
+        <v>916</v>
       </c>
       <c r="AX3">
-        <v>0.36</v>
+        <v>0.67</v>
       </c>
       <c r="AY3">
         <v>224223560</v>
       </c>
       <c r="AZ3">
-        <v>155975</v>
+        <v>92528</v>
       </c>
       <c r="BA3">
         <v>51</v>
@@ -1016,10 +1016,10 @@
         <v>202</v>
       </c>
       <c r="BD3">
-        <v>247</v>
+        <v>227</v>
       </c>
       <c r="BE3">
-        <v>1470</v>
+        <v>793</v>
       </c>
       <c r="BF3" t="b">
         <v>1</v>
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>12.5</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>0.8</v>
@@ -1041,10 +1041,10 @@
         <v>6</v>
       </c>
       <c r="E4">
-        <v>12.5</v>
+        <v>14</v>
       </c>
       <c r="F4">
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>90</v>
@@ -1116,98 +1116,98 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>356 x 171 x 57</t>
+          <t>457 x 152 x 60</t>
         </is>
       </c>
       <c r="AB4">
         <v>355</v>
       </c>
       <c r="AC4">
-        <v>5155</v>
+        <v>5410</v>
       </c>
       <c r="AD4">
-        <v>3316</v>
+        <v>4213</v>
       </c>
       <c r="AE4">
-        <v>1.25</v>
+        <v>1.13</v>
       </c>
       <c r="AF4">
         <v>0.21</v>
       </c>
       <c r="AG4">
-        <v>0.5</v>
+        <v>0.57</v>
       </c>
       <c r="AH4">
-        <v>2584</v>
+        <v>3103</v>
       </c>
       <c r="AI4">
         <v>355</v>
       </c>
       <c r="AJ4">
-        <v>5155</v>
+        <v>5410</v>
       </c>
       <c r="AK4">
-        <v>363000</v>
+        <v>381000</v>
       </c>
       <c r="AL4">
-        <v>75236</v>
+        <v>73009</v>
       </c>
       <c r="AM4">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="AN4">
         <v>0.21</v>
       </c>
       <c r="AO4">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="AP4">
-        <v>5084</v>
+        <v>5323</v>
       </c>
       <c r="AQ4">
         <v>355</v>
       </c>
       <c r="AR4">
-        <v>2577</v>
+        <v>2705</v>
       </c>
       <c r="AS4">
-        <v>35947</v>
+        <v>25746</v>
       </c>
       <c r="AT4">
-        <v>0.27</v>
+        <v>0.32</v>
       </c>
       <c r="AU4">
         <v>0.21</v>
       </c>
       <c r="AV4">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
       <c r="AW4">
-        <v>2538</v>
+        <v>2629</v>
       </c>
       <c r="AX4">
-        <v>0.5600000000000001</v>
+        <v>1.04</v>
       </c>
       <c r="AY4">
         <v>224223560</v>
       </c>
       <c r="AZ4">
-        <v>75236</v>
+        <v>62952</v>
       </c>
       <c r="BA4">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB4">
-        <v>382</v>
+        <v>437</v>
       </c>
       <c r="BC4">
-        <v>640</v>
+        <v>817</v>
       </c>
       <c r="BD4">
-        <v>806</v>
+        <v>1023</v>
       </c>
       <c r="BE4">
-        <v>2410</v>
+        <v>2431</v>
       </c>
       <c r="BF4" t="b">
         <v>1</v>
@@ -1265,7 +1265,7 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q5">
-        <v>4658</v>
+        <v>2470</v>
       </c>
       <c r="R5">
         <v>50</v>
@@ -1299,46 +1299,46 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>4658</t>
+          <t>2470</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>406 x 178 x 54</t>
+          <t>203 x 133 x 30</t>
         </is>
       </c>
       <c r="AB5">
         <v>355</v>
       </c>
       <c r="AC5">
-        <v>4899</v>
+        <v>2712</v>
       </c>
       <c r="AD5">
-        <v>12359</v>
+        <v>1917</v>
       </c>
       <c r="AE5">
-        <v>0.63</v>
+        <v>1.19</v>
       </c>
       <c r="AF5">
         <v>0.21</v>
       </c>
       <c r="AG5">
-        <v>0.88</v>
+        <v>0.54</v>
       </c>
       <c r="AH5">
-        <v>4303</v>
+        <v>1455</v>
       </c>
       <c r="AI5">
         <v>355</v>
       </c>
       <c r="AJ5">
-        <v>4899</v>
+        <v>2712</v>
       </c>
       <c r="AK5">
-        <v>345000</v>
+        <v>191000</v>
       </c>
       <c r="AL5">
-        <v>228014</v>
+        <v>126234</v>
       </c>
       <c r="AM5">
         <v>0.15</v>
@@ -1350,37 +1350,37 @@
         <v>1.01</v>
       </c>
       <c r="AP5">
-        <v>4956</v>
+        <v>2744</v>
       </c>
       <c r="AQ5">
         <v>355</v>
       </c>
       <c r="AR5">
-        <v>2450</v>
+        <v>1356</v>
       </c>
       <c r="AS5">
-        <v>33032</v>
+        <v>12468</v>
       </c>
       <c r="AT5">
-        <v>0.27</v>
+        <v>0.33</v>
       </c>
       <c r="AU5">
         <v>0.21</v>
       </c>
       <c r="AV5">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
       <c r="AW5">
-        <v>2410</v>
+        <v>1316</v>
       </c>
       <c r="AX5">
-        <v>0.53</v>
+        <v>0.75</v>
       </c>
       <c r="AY5">
         <v>224223560</v>
       </c>
       <c r="AZ5">
-        <v>228014</v>
+        <v>126234</v>
       </c>
       <c r="BA5">
         <v>51</v>
@@ -1392,10 +1392,10 @@
         <v>202</v>
       </c>
       <c r="BD5">
-        <v>273</v>
+        <v>241</v>
       </c>
       <c r="BE5">
-        <v>2356</v>
+        <v>1259</v>
       </c>
       <c r="BF5" t="b">
         <v>1</v>
@@ -1408,7 +1408,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>12.5</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>0.8</v>
@@ -1417,10 +1417,10 @@
         <v>6</v>
       </c>
       <c r="E6">
-        <v>12.5</v>
+        <v>14</v>
       </c>
       <c r="F6">
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="G6">
         <v>90</v>
@@ -1435,7 +1435,7 @@
         <v>2</v>
       </c>
       <c r="K6">
-        <v>2270</v>
+        <v>1510</v>
       </c>
       <c r="L6">
         <v>210</v>
@@ -1450,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="P6">
-        <v>17.8</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="Q6">
         <v>7849</v>
@@ -1502,19 +1502,19 @@
         <v>8307</v>
       </c>
       <c r="AD6">
-        <v>13389</v>
+        <v>10674</v>
       </c>
       <c r="AE6">
-        <v>0.79</v>
+        <v>0.88</v>
       </c>
       <c r="AF6">
         <v>0.21</v>
       </c>
       <c r="AG6">
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="AH6">
-        <v>6668</v>
+        <v>6193</v>
       </c>
       <c r="AI6">
         <v>355</v>
@@ -1526,19 +1526,19 @@
         <v>585000</v>
       </c>
       <c r="AL6">
-        <v>121248</v>
+        <v>112101</v>
       </c>
       <c r="AM6">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="AN6">
         <v>0.21</v>
       </c>
       <c r="AO6">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="AP6">
-        <v>8193</v>
+        <v>8173</v>
       </c>
       <c r="AQ6">
         <v>355</v>
@@ -1562,28 +1562,28 @@
         <v>4062</v>
       </c>
       <c r="AX6">
-        <v>0.9</v>
+        <v>1.36</v>
       </c>
       <c r="AY6">
-        <v>337077803</v>
+        <v>224223560</v>
       </c>
       <c r="AZ6">
-        <v>121248</v>
+        <v>96658</v>
       </c>
       <c r="BA6">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB6">
-        <v>382</v>
+        <v>437</v>
       </c>
       <c r="BC6">
-        <v>640</v>
+        <v>817</v>
       </c>
       <c r="BD6">
-        <v>907</v>
+        <v>1128</v>
       </c>
       <c r="BE6">
-        <v>4015</v>
+        <v>4037</v>
       </c>
       <c r="BF6" t="b">
         <v>1</v>
@@ -1623,7 +1623,7 @@
         <v>2</v>
       </c>
       <c r="K7">
-        <v>2270</v>
+        <v>1510</v>
       </c>
       <c r="L7">
         <v>210</v>
@@ -1638,10 +1638,10 @@
         <v>1</v>
       </c>
       <c r="P7">
-        <v>17.8</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="Q7">
-        <v>7849</v>
+        <v>4162</v>
       </c>
       <c r="R7">
         <v>50</v>
@@ -1675,46 +1675,46 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>7849</t>
+          <t>4162</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>610 x 178 x 92</t>
+          <t>356 x 171 x 51</t>
         </is>
       </c>
       <c r="AB7">
         <v>355</v>
       </c>
       <c r="AC7">
-        <v>8307</v>
+        <v>4608</v>
       </c>
       <c r="AD7">
-        <v>42695</v>
+        <v>9319</v>
       </c>
       <c r="AE7">
-        <v>0.44</v>
+        <v>0.7</v>
       </c>
       <c r="AF7">
         <v>0.21</v>
       </c>
       <c r="AG7">
-        <v>0.9399999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="AH7">
-        <v>7822</v>
+        <v>3899</v>
       </c>
       <c r="AI7">
         <v>355</v>
       </c>
       <c r="AJ7">
-        <v>8307</v>
+        <v>4608</v>
       </c>
       <c r="AK7">
-        <v>585000</v>
+        <v>324500</v>
       </c>
       <c r="AL7">
-        <v>386633</v>
+        <v>214466</v>
       </c>
       <c r="AM7">
         <v>0.15</v>
@@ -1726,19 +1726,19 @@
         <v>1.01</v>
       </c>
       <c r="AP7">
-        <v>8403</v>
+        <v>4661</v>
       </c>
       <c r="AQ7">
         <v>355</v>
       </c>
       <c r="AR7">
-        <v>4154</v>
+        <v>2304</v>
       </c>
       <c r="AS7">
-        <v>46634</v>
+        <v>31348</v>
       </c>
       <c r="AT7">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
       <c r="AU7">
         <v>0.21</v>
@@ -1747,31 +1747,31 @@
         <v>0.98</v>
       </c>
       <c r="AW7">
-        <v>4062</v>
+        <v>2267</v>
       </c>
       <c r="AX7">
-        <v>0.9</v>
+        <v>0.96</v>
       </c>
       <c r="AY7">
-        <v>337077803</v>
+        <v>224223560</v>
       </c>
       <c r="AZ7">
-        <v>386633</v>
+        <v>214466</v>
       </c>
       <c r="BA7">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB7">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="BC7">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="BD7">
-        <v>322</v>
+        <v>270</v>
       </c>
       <c r="BE7">
-        <v>3957</v>
+        <v>2108</v>
       </c>
       <c r="BF7" t="b">
         <v>1</v>
@@ -1784,7 +1784,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>12.5</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <v>0.8</v>
@@ -1793,10 +1793,10 @@
         <v>6</v>
       </c>
       <c r="E8">
-        <v>12.5</v>
+        <v>14</v>
       </c>
       <c r="F8">
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="G8">
         <v>90</v>
@@ -1811,7 +1811,7 @@
         <v>2</v>
       </c>
       <c r="K8">
-        <v>2270</v>
+        <v>1510</v>
       </c>
       <c r="L8">
         <v>210</v>
@@ -1826,7 +1826,7 @@
         <v>1</v>
       </c>
       <c r="P8">
-        <v>17.8</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="Q8">
         <v>6898</v>
@@ -1878,19 +1878,19 @@
         <v>7384</v>
       </c>
       <c r="AD8">
-        <v>11586</v>
+        <v>9236</v>
       </c>
       <c r="AE8">
-        <v>0.8</v>
+        <v>0.89</v>
       </c>
       <c r="AF8">
         <v>0.21</v>
       </c>
       <c r="AG8">
-        <v>0.8</v>
+        <v>0.74</v>
       </c>
       <c r="AH8">
-        <v>5883</v>
+        <v>5448</v>
       </c>
       <c r="AI8">
         <v>355</v>
@@ -1902,19 +1902,19 @@
         <v>520000</v>
       </c>
       <c r="AL8">
-        <v>107776</v>
+        <v>99645</v>
       </c>
       <c r="AM8">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="AN8">
         <v>0.21</v>
       </c>
       <c r="AO8">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="AP8">
-        <v>7283</v>
+        <v>7265</v>
       </c>
       <c r="AQ8">
         <v>355</v>
@@ -1938,28 +1938,28 @@
         <v>3603</v>
       </c>
       <c r="AX8">
-        <v>0.8</v>
+        <v>1.26</v>
       </c>
       <c r="AY8">
-        <v>337077803</v>
+        <v>224223560</v>
       </c>
       <c r="AZ8">
-        <v>107776</v>
+        <v>85918</v>
       </c>
       <c r="BA8">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB8">
-        <v>382</v>
+        <v>437</v>
       </c>
       <c r="BC8">
-        <v>640</v>
+        <v>817</v>
       </c>
       <c r="BD8">
-        <v>881</v>
+        <v>1098</v>
       </c>
       <c r="BE8">
-        <v>3537</v>
+        <v>3559</v>
       </c>
       <c r="BF8" t="b">
         <v>1</v>
@@ -1999,7 +1999,7 @@
         <v>2</v>
       </c>
       <c r="K9">
-        <v>2270</v>
+        <v>1510</v>
       </c>
       <c r="L9">
         <v>210</v>
@@ -2014,10 +2014,10 @@
         <v>1</v>
       </c>
       <c r="P9">
-        <v>17.8</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="Q9">
-        <v>6898</v>
+        <v>3658</v>
       </c>
       <c r="R9">
         <v>50</v>
@@ -2051,46 +2051,46 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>6898</t>
+          <t>3658</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>610 x 178 x 82</t>
+          <t>254 x 146 x 43</t>
         </is>
       </c>
       <c r="AB9">
         <v>355</v>
       </c>
       <c r="AC9">
-        <v>7384</v>
+        <v>3891</v>
       </c>
       <c r="AD9">
-        <v>36945</v>
+        <v>4322</v>
       </c>
       <c r="AE9">
-        <v>0.45</v>
+        <v>0.95</v>
       </c>
       <c r="AF9">
         <v>0.21</v>
       </c>
       <c r="AG9">
-        <v>0.9399999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="AH9">
-        <v>6941</v>
+        <v>2728</v>
       </c>
       <c r="AI9">
         <v>355</v>
       </c>
       <c r="AJ9">
-        <v>7384</v>
+        <v>3891</v>
       </c>
       <c r="AK9">
-        <v>520000</v>
+        <v>274000</v>
       </c>
       <c r="AL9">
-        <v>343674</v>
+        <v>181090</v>
       </c>
       <c r="AM9">
         <v>0.15</v>
@@ -2102,19 +2102,19 @@
         <v>1.01</v>
       </c>
       <c r="AP9">
-        <v>7470</v>
+        <v>3936</v>
       </c>
       <c r="AQ9">
         <v>355</v>
       </c>
       <c r="AR9">
-        <v>3692</v>
+        <v>1945</v>
       </c>
       <c r="AS9">
-        <v>39185</v>
+        <v>21924</v>
       </c>
       <c r="AT9">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
       <c r="AU9">
         <v>0.21</v>
@@ -2123,31 +2123,31 @@
         <v>0.98</v>
       </c>
       <c r="AW9">
-        <v>3603</v>
+        <v>1903</v>
       </c>
       <c r="AX9">
-        <v>0.8</v>
+        <v>0.88</v>
       </c>
       <c r="AY9">
-        <v>337077803</v>
+        <v>224223560</v>
       </c>
       <c r="AZ9">
-        <v>343674</v>
+        <v>181090</v>
       </c>
       <c r="BA9">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB9">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="BC9">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="BD9">
-        <v>309</v>
+        <v>263</v>
       </c>
       <c r="BE9">
-        <v>3480</v>
+        <v>1855</v>
       </c>
       <c r="BF9" t="b">
         <v>1</v>
@@ -2160,7 +2160,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>12.5</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>0.8</v>
@@ -2169,10 +2169,10 @@
         <v>6</v>
       </c>
       <c r="E10">
-        <v>12.5</v>
+        <v>14</v>
       </c>
       <c r="F10">
-        <v>12.5</v>
+        <v>13</v>
       </c>
       <c r="G10">
         <v>90</v>
@@ -2187,7 +2187,7 @@
         <v>2</v>
       </c>
       <c r="K10">
-        <v>2270</v>
+        <v>1510</v>
       </c>
       <c r="L10">
         <v>210</v>
@@ -2202,7 +2202,7 @@
         <v>1</v>
       </c>
       <c r="P10">
-        <v>17.8</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="Q10">
         <v>3843</v>
@@ -2244,65 +2244,65 @@
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>406 x 140 x 46</t>
+          <t>457 x 152 x 52</t>
         </is>
       </c>
       <c r="AB10">
         <v>355</v>
       </c>
       <c r="AC10">
-        <v>4161</v>
+        <v>4729</v>
       </c>
       <c r="AD10">
-        <v>3254</v>
+        <v>3536</v>
       </c>
       <c r="AE10">
-        <v>1.13</v>
+        <v>1.16</v>
       </c>
       <c r="AF10">
         <v>0.21</v>
       </c>
       <c r="AG10">
-        <v>0.58</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="AH10">
-        <v>2393</v>
+        <v>2639</v>
       </c>
       <c r="AI10">
         <v>355</v>
       </c>
       <c r="AJ10">
-        <v>4161</v>
+        <v>4729</v>
       </c>
       <c r="AK10">
-        <v>293000</v>
+        <v>333000</v>
       </c>
       <c r="AL10">
-        <v>60728</v>
+        <v>63811</v>
       </c>
       <c r="AM10">
-        <v>0.26</v>
+        <v>0.27</v>
       </c>
       <c r="AN10">
         <v>0.21</v>
       </c>
       <c r="AO10">
-        <v>0.99</v>
+        <v>0.98</v>
       </c>
       <c r="AP10">
-        <v>4104</v>
+        <v>4652</v>
       </c>
       <c r="AQ10">
         <v>355</v>
       </c>
       <c r="AR10">
-        <v>2080</v>
+        <v>2364</v>
       </c>
       <c r="AS10">
-        <v>17423</v>
+        <v>20888</v>
       </c>
       <c r="AT10">
-        <v>0.35</v>
+        <v>0.34</v>
       </c>
       <c r="AU10">
         <v>0.21</v>
@@ -2311,31 +2311,31 @@
         <v>0.97</v>
       </c>
       <c r="AW10">
-        <v>2011</v>
+        <v>2291</v>
       </c>
       <c r="AX10">
-        <v>0.45</v>
+        <v>0.97</v>
       </c>
       <c r="AY10">
-        <v>337077803</v>
+        <v>224223560</v>
       </c>
       <c r="AZ10">
-        <v>60728</v>
+        <v>55021</v>
       </c>
       <c r="BA10">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB10">
-        <v>382</v>
+        <v>437</v>
       </c>
       <c r="BC10">
-        <v>640</v>
+        <v>817</v>
       </c>
       <c r="BD10">
-        <v>786</v>
+        <v>994</v>
       </c>
       <c r="BE10">
-        <v>2000</v>
+        <v>2021</v>
       </c>
       <c r="BF10" t="b">
         <v>1</v>
@@ -2375,7 +2375,7 @@
         <v>2</v>
       </c>
       <c r="K11">
-        <v>2270</v>
+        <v>1510</v>
       </c>
       <c r="L11">
         <v>210</v>
@@ -2390,10 +2390,10 @@
         <v>1</v>
       </c>
       <c r="P11">
-        <v>17.8</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="Q11">
-        <v>3843</v>
+        <v>2038</v>
       </c>
       <c r="R11">
         <v>50</v>
@@ -2427,46 +2427,46 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>3843</t>
+          <t>2038</t>
         </is>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>356 x 171 x 45</t>
+          <t>254 x 102 x 25</t>
         </is>
       </c>
       <c r="AB11">
         <v>355</v>
       </c>
       <c r="AC11">
-        <v>4068</v>
+        <v>2272</v>
       </c>
       <c r="AD11">
-        <v>7997</v>
+        <v>2254</v>
       </c>
       <c r="AE11">
-        <v>0.71</v>
+        <v>1</v>
       </c>
       <c r="AF11">
         <v>0.21</v>
       </c>
       <c r="AG11">
-        <v>0.84</v>
+        <v>0.66</v>
       </c>
       <c r="AH11">
-        <v>3423</v>
+        <v>1506</v>
       </c>
       <c r="AI11">
         <v>355</v>
       </c>
       <c r="AJ11">
-        <v>4068</v>
+        <v>2272</v>
       </c>
       <c r="AK11">
-        <v>286500</v>
+        <v>160000</v>
       </c>
       <c r="AL11">
-        <v>189351</v>
+        <v>105746</v>
       </c>
       <c r="AM11">
         <v>0.15</v>
@@ -2478,37 +2478,37 @@
         <v>1.01</v>
       </c>
       <c r="AP11">
-        <v>4115</v>
+        <v>2298</v>
       </c>
       <c r="AQ11">
         <v>355</v>
       </c>
       <c r="AR11">
-        <v>2034</v>
+        <v>1136</v>
       </c>
       <c r="AS11">
-        <v>26264</v>
+        <v>4825</v>
       </c>
       <c r="AT11">
-        <v>0.28</v>
+        <v>0.49</v>
       </c>
       <c r="AU11">
         <v>0.21</v>
       </c>
       <c r="AV11">
-        <v>0.98</v>
+        <v>0.93</v>
       </c>
       <c r="AW11">
-        <v>1999</v>
+        <v>1055</v>
       </c>
       <c r="AX11">
-        <v>0.44</v>
+        <v>0.7</v>
       </c>
       <c r="AY11">
-        <v>337077803</v>
+        <v>224223560</v>
       </c>
       <c r="AZ11">
-        <v>189351</v>
+        <v>105746</v>
       </c>
       <c r="BA11">
         <v>51</v>
@@ -2520,10 +2520,10 @@
         <v>202</v>
       </c>
       <c r="BD11">
-        <v>261</v>
+        <v>235</v>
       </c>
       <c r="BE11">
-        <v>1948</v>
+        <v>1042</v>
       </c>
       <c r="BF11" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
correcting formula for check #4
</commit_message>
<xml_diff>
--- a/tables/input/output_processed_table.xlsx
+++ b/tables/input/output_processed_table.xlsx
@@ -701,7 +701,7 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q2">
-        <v>2748</v>
+        <v>2915</v>
       </c>
       <c r="R2">
         <v>50</v>
@@ -730,51 +730,51 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>150</t>
+          <t>286</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>2898</t>
+          <t>3202</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>406 x 140 x 39</t>
+          <t>457 x 191 x 74</t>
         </is>
       </c>
       <c r="AB2">
         <v>355</v>
       </c>
       <c r="AC2">
-        <v>3529</v>
+        <v>6717</v>
       </c>
       <c r="AD2">
-        <v>2065</v>
+        <v>5502</v>
       </c>
       <c r="AE2">
-        <v>1.31</v>
+        <v>1.1</v>
       </c>
       <c r="AF2">
         <v>0.21</v>
       </c>
       <c r="AG2">
-        <v>0.47</v>
+        <v>0.59</v>
       </c>
       <c r="AH2">
-        <v>1646</v>
+        <v>3981</v>
       </c>
       <c r="AI2">
         <v>355</v>
       </c>
       <c r="AJ2">
-        <v>3529</v>
+        <v>6717</v>
       </c>
       <c r="AK2">
-        <v>248500</v>
+        <v>473000</v>
       </c>
       <c r="AL2">
-        <v>47619</v>
+        <v>90639</v>
       </c>
       <c r="AM2">
         <v>0.27</v>
@@ -786,37 +786,37 @@
         <v>0.98</v>
       </c>
       <c r="AP2">
-        <v>3472</v>
+        <v>6608</v>
       </c>
       <c r="AQ2">
         <v>355</v>
       </c>
       <c r="AR2">
-        <v>1764</v>
+        <v>3358</v>
       </c>
       <c r="AS2">
-        <v>13278</v>
+        <v>54082</v>
       </c>
       <c r="AT2">
-        <v>0.36</v>
+        <v>0.25</v>
       </c>
       <c r="AU2">
         <v>0.21</v>
       </c>
       <c r="AV2">
-        <v>0.96</v>
+        <v>0.99</v>
       </c>
       <c r="AW2">
-        <v>1697</v>
+        <v>3322</v>
       </c>
       <c r="AX2">
-        <v>0.84</v>
+        <v>1.18</v>
       </c>
       <c r="AY2">
         <v>224223560</v>
       </c>
       <c r="AZ2">
-        <v>41059</v>
+        <v>78153</v>
       </c>
       <c r="BA2">
         <v>52</v>
@@ -828,10 +828,10 @@
         <v>817</v>
       </c>
       <c r="BD2">
-        <v>966</v>
+        <v>1085</v>
       </c>
       <c r="BE2">
-        <v>1546</v>
+        <v>3310</v>
       </c>
       <c r="BF2" t="b">
         <v>1</v>
@@ -889,7 +889,7 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q3">
-        <v>1457</v>
+        <v>1546</v>
       </c>
       <c r="R3">
         <v>50</v>
@@ -918,51 +918,51 @@
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>84</t>
+          <t>154</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>1541</t>
+          <t>1700</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>254 x 102 x 22</t>
+          <t>305 x 165 x 40</t>
         </is>
       </c>
       <c r="AB3">
         <v>355</v>
       </c>
       <c r="AC3">
-        <v>1988</v>
+        <v>3642</v>
       </c>
       <c r="AD3">
-        <v>1877</v>
+        <v>5618</v>
       </c>
       <c r="AE3">
-        <v>1.03</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="AF3">
         <v>0.21</v>
       </c>
       <c r="AG3">
-        <v>0.65</v>
+        <v>0.79</v>
       </c>
       <c r="AH3">
-        <v>1283</v>
+        <v>2887</v>
       </c>
       <c r="AI3">
         <v>355</v>
       </c>
       <c r="AJ3">
-        <v>1988</v>
+        <v>3642</v>
       </c>
       <c r="AK3">
-        <v>140000</v>
+        <v>256500</v>
       </c>
       <c r="AL3">
-        <v>92528</v>
+        <v>169524</v>
       </c>
       <c r="AM3">
         <v>0.15</v>
@@ -974,52 +974,52 @@
         <v>1.01</v>
       </c>
       <c r="AP3">
-        <v>2011</v>
+        <v>3685</v>
       </c>
       <c r="AQ3">
         <v>355</v>
       </c>
       <c r="AR3">
-        <v>994</v>
+        <v>1821</v>
       </c>
       <c r="AS3">
-        <v>3854</v>
+        <v>24742</v>
       </c>
       <c r="AT3">
-        <v>0.51</v>
+        <v>0.27</v>
       </c>
       <c r="AU3">
         <v>0.21</v>
       </c>
       <c r="AV3">
-        <v>0.92</v>
+        <v>0.98</v>
       </c>
       <c r="AW3">
-        <v>916</v>
+        <v>1792</v>
       </c>
       <c r="AX3">
-        <v>0.67</v>
+        <v>0.85</v>
       </c>
       <c r="AY3">
         <v>224223560</v>
       </c>
       <c r="AZ3">
-        <v>92528</v>
+        <v>169524</v>
       </c>
       <c r="BA3">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB3">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="BC3">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="BD3">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="BE3">
-        <v>793</v>
+        <v>1726</v>
       </c>
       <c r="BF3" t="b">
         <v>1</v>
@@ -1077,7 +1077,7 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q4">
-        <v>4658</v>
+        <v>4810</v>
       </c>
       <c r="R4">
         <v>50</v>
@@ -1111,46 +1111,46 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>4658</t>
+          <t>4810</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>457 x 152 x 60</t>
+          <t>610 x 229 x 113</t>
         </is>
       </c>
       <c r="AB4">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AC4">
-        <v>5410</v>
+        <v>9936</v>
       </c>
       <c r="AD4">
-        <v>4213</v>
+        <v>14424</v>
       </c>
       <c r="AE4">
-        <v>1.13</v>
+        <v>0.83</v>
       </c>
       <c r="AF4">
         <v>0.21</v>
       </c>
       <c r="AG4">
-        <v>0.57</v>
+        <v>0.78</v>
       </c>
       <c r="AH4">
-        <v>3103</v>
+        <v>7732</v>
       </c>
       <c r="AI4">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AJ4">
-        <v>5410</v>
+        <v>9936</v>
       </c>
       <c r="AK4">
-        <v>381000</v>
+        <v>720000</v>
       </c>
       <c r="AL4">
-        <v>73009</v>
+        <v>137970</v>
       </c>
       <c r="AM4">
         <v>0.27</v>
@@ -1162,37 +1162,37 @@
         <v>0.98</v>
       </c>
       <c r="AP4">
-        <v>5323</v>
+        <v>9785</v>
       </c>
       <c r="AQ4">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AR4">
-        <v>2705</v>
+        <v>4968</v>
       </c>
       <c r="AS4">
-        <v>25746</v>
+        <v>111079</v>
       </c>
       <c r="AT4">
-        <v>0.32</v>
+        <v>0.21</v>
       </c>
       <c r="AU4">
         <v>0.21</v>
       </c>
       <c r="AV4">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="AW4">
-        <v>2629</v>
+        <v>4955</v>
       </c>
       <c r="AX4">
-        <v>1.04</v>
+        <v>1.56</v>
       </c>
       <c r="AY4">
         <v>224223560</v>
       </c>
       <c r="AZ4">
-        <v>62952</v>
+        <v>118964</v>
       </c>
       <c r="BA4">
         <v>52</v>
@@ -1204,10 +1204,10 @@
         <v>817</v>
       </c>
       <c r="BD4">
-        <v>1023</v>
+        <v>1182</v>
       </c>
       <c r="BE4">
-        <v>2431</v>
+        <v>4928</v>
       </c>
       <c r="BF4" t="b">
         <v>1</v>
@@ -1265,7 +1265,7 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q5">
-        <v>2470</v>
+        <v>2551</v>
       </c>
       <c r="R5">
         <v>50</v>
@@ -1299,46 +1299,46 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>2470</t>
+          <t>2551</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>203 x 133 x 30</t>
+          <t>457 x 152 x 60</t>
         </is>
       </c>
       <c r="AB5">
         <v>355</v>
       </c>
       <c r="AC5">
-        <v>2712</v>
+        <v>5410</v>
       </c>
       <c r="AD5">
-        <v>1917</v>
+        <v>16853</v>
       </c>
       <c r="AE5">
-        <v>1.19</v>
+        <v>0.57</v>
       </c>
       <c r="AF5">
         <v>0.21</v>
       </c>
       <c r="AG5">
-        <v>0.54</v>
+        <v>0.9</v>
       </c>
       <c r="AH5">
-        <v>1455</v>
+        <v>4881</v>
       </c>
       <c r="AI5">
         <v>355</v>
       </c>
       <c r="AJ5">
-        <v>2712</v>
+        <v>5410</v>
       </c>
       <c r="AK5">
-        <v>191000</v>
+        <v>381000</v>
       </c>
       <c r="AL5">
-        <v>126234</v>
+        <v>251807</v>
       </c>
       <c r="AM5">
         <v>0.15</v>
@@ -1350,19 +1350,19 @@
         <v>1.01</v>
       </c>
       <c r="AP5">
-        <v>2744</v>
+        <v>5473</v>
       </c>
       <c r="AQ5">
         <v>355</v>
       </c>
       <c r="AR5">
-        <v>1356</v>
+        <v>2705</v>
       </c>
       <c r="AS5">
-        <v>12468</v>
+        <v>25746</v>
       </c>
       <c r="AT5">
-        <v>0.33</v>
+        <v>0.32</v>
       </c>
       <c r="AU5">
         <v>0.21</v>
@@ -1371,31 +1371,31 @@
         <v>0.97</v>
       </c>
       <c r="AW5">
-        <v>1316</v>
+        <v>2629</v>
       </c>
       <c r="AX5">
-        <v>0.75</v>
+        <v>1.04</v>
       </c>
       <c r="AY5">
         <v>224223560</v>
       </c>
       <c r="AZ5">
-        <v>126234</v>
+        <v>251807</v>
       </c>
       <c r="BA5">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB5">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="BC5">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="BD5">
-        <v>241</v>
+        <v>283</v>
       </c>
       <c r="BE5">
-        <v>1259</v>
+        <v>2579</v>
       </c>
       <c r="BF5" t="b">
         <v>1</v>
@@ -1453,7 +1453,7 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q6">
-        <v>7849</v>
+        <v>6885</v>
       </c>
       <c r="R6">
         <v>50</v>
@@ -1487,46 +1487,46 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>7849</t>
+          <t>6885</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>610 x 178 x 92</t>
+          <t>457 x 191 x 161</t>
         </is>
       </c>
       <c r="AB6">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AC6">
-        <v>8307</v>
+        <v>14214</v>
       </c>
       <c r="AD6">
-        <v>10674</v>
+        <v>13185</v>
       </c>
       <c r="AE6">
-        <v>0.88</v>
+        <v>1.04</v>
       </c>
       <c r="AF6">
         <v>0.21</v>
       </c>
       <c r="AG6">
-        <v>0.75</v>
+        <v>0.64</v>
       </c>
       <c r="AH6">
-        <v>6193</v>
+        <v>9080</v>
       </c>
       <c r="AI6">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AJ6">
-        <v>8307</v>
+        <v>14214</v>
       </c>
       <c r="AK6">
-        <v>585000</v>
+        <v>1030000</v>
       </c>
       <c r="AL6">
-        <v>112101</v>
+        <v>197374</v>
       </c>
       <c r="AM6">
         <v>0.27</v>
@@ -1538,52 +1538,52 @@
         <v>0.98</v>
       </c>
       <c r="AP6">
-        <v>8173</v>
+        <v>13998</v>
       </c>
       <c r="AQ6">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AR6">
-        <v>4154</v>
+        <v>7107</v>
       </c>
       <c r="AS6">
-        <v>46634</v>
+        <v>137635</v>
       </c>
       <c r="AT6">
-        <v>0.3</v>
+        <v>0.23</v>
       </c>
       <c r="AU6">
         <v>0.21</v>
       </c>
       <c r="AV6">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="AW6">
-        <v>4062</v>
+        <v>7064</v>
       </c>
       <c r="AX6">
-        <v>1.36</v>
+        <v>2.03</v>
       </c>
       <c r="AY6">
         <v>224223560</v>
       </c>
       <c r="AZ6">
-        <v>96658</v>
+        <v>170185</v>
       </c>
       <c r="BA6">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="BB6">
-        <v>437</v>
+        <v>445</v>
       </c>
       <c r="BC6">
-        <v>817</v>
+        <v>833</v>
       </c>
       <c r="BD6">
-        <v>1128</v>
+        <v>1326</v>
       </c>
       <c r="BE6">
-        <v>4037</v>
+        <v>7018</v>
       </c>
       <c r="BF6" t="b">
         <v>1</v>
@@ -1641,7 +1641,7 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q7">
-        <v>4162</v>
+        <v>3651</v>
       </c>
       <c r="R7">
         <v>50</v>
@@ -1675,46 +1675,46 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>4162</t>
+          <t>3651</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>356 x 171 x 51</t>
+          <t>533 x 210 x 82</t>
         </is>
       </c>
       <c r="AB7">
         <v>355</v>
       </c>
       <c r="AC7">
-        <v>4608</v>
+        <v>7455</v>
       </c>
       <c r="AD7">
-        <v>9319</v>
+        <v>31393</v>
       </c>
       <c r="AE7">
-        <v>0.7</v>
+        <v>0.49</v>
       </c>
       <c r="AF7">
         <v>0.21</v>
       </c>
       <c r="AG7">
-        <v>0.85</v>
+        <v>0.93</v>
       </c>
       <c r="AH7">
-        <v>3899</v>
+        <v>6919</v>
       </c>
       <c r="AI7">
         <v>355</v>
       </c>
       <c r="AJ7">
-        <v>4608</v>
+        <v>7455</v>
       </c>
       <c r="AK7">
-        <v>324500</v>
+        <v>525000</v>
       </c>
       <c r="AL7">
-        <v>214466</v>
+        <v>346978</v>
       </c>
       <c r="AM7">
         <v>0.15</v>
@@ -1726,37 +1726,37 @@
         <v>1.01</v>
       </c>
       <c r="AP7">
-        <v>4661</v>
+        <v>7541</v>
       </c>
       <c r="AQ7">
         <v>355</v>
       </c>
       <c r="AR7">
-        <v>2304</v>
+        <v>3728</v>
       </c>
       <c r="AS7">
-        <v>31348</v>
+        <v>65093</v>
       </c>
       <c r="AT7">
-        <v>0.27</v>
+        <v>0.24</v>
       </c>
       <c r="AU7">
         <v>0.21</v>
       </c>
       <c r="AV7">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="AW7">
-        <v>2267</v>
+        <v>3695</v>
       </c>
       <c r="AX7">
-        <v>0.96</v>
+        <v>1.26</v>
       </c>
       <c r="AY7">
         <v>224223560</v>
       </c>
       <c r="AZ7">
-        <v>214466</v>
+        <v>346978</v>
       </c>
       <c r="BA7">
         <v>52</v>
@@ -1768,10 +1768,10 @@
         <v>206</v>
       </c>
       <c r="BD7">
-        <v>270</v>
+        <v>315</v>
       </c>
       <c r="BE7">
-        <v>2108</v>
+        <v>3682</v>
       </c>
       <c r="BF7" t="b">
         <v>1</v>
@@ -1829,7 +1829,7 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q8">
-        <v>6898</v>
+        <v>5704</v>
       </c>
       <c r="R8">
         <v>50</v>
@@ -1863,46 +1863,46 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>6898</t>
+          <t>5704</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>610 x 178 x 82</t>
+          <t>762 x 267 x 134</t>
         </is>
       </c>
       <c r="AB8">
         <v>355</v>
       </c>
       <c r="AC8">
-        <v>7384</v>
+        <v>12141</v>
       </c>
       <c r="AD8">
-        <v>9236</v>
+        <v>24949</v>
       </c>
       <c r="AE8">
-        <v>0.89</v>
+        <v>0.7</v>
       </c>
       <c r="AF8">
         <v>0.21</v>
       </c>
       <c r="AG8">
-        <v>0.74</v>
+        <v>0.85</v>
       </c>
       <c r="AH8">
-        <v>5448</v>
+        <v>10306</v>
       </c>
       <c r="AI8">
         <v>355</v>
       </c>
       <c r="AJ8">
-        <v>7384</v>
+        <v>12141</v>
       </c>
       <c r="AK8">
-        <v>520000</v>
+        <v>855000</v>
       </c>
       <c r="AL8">
-        <v>99645</v>
+        <v>163839</v>
       </c>
       <c r="AM8">
         <v>0.27</v>
@@ -1914,37 +1914,37 @@
         <v>0.98</v>
       </c>
       <c r="AP8">
-        <v>7265</v>
+        <v>11946</v>
       </c>
       <c r="AQ8">
         <v>355</v>
       </c>
       <c r="AR8">
-        <v>3692</v>
+        <v>6070</v>
       </c>
       <c r="AS8">
-        <v>39185</v>
+        <v>155122</v>
       </c>
       <c r="AT8">
-        <v>0.31</v>
+        <v>0.2</v>
       </c>
       <c r="AU8">
         <v>0.21</v>
       </c>
       <c r="AV8">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="AW8">
-        <v>3603</v>
+        <v>6073</v>
       </c>
       <c r="AX8">
-        <v>1.26</v>
+        <v>1.77</v>
       </c>
       <c r="AY8">
         <v>224223560</v>
       </c>
       <c r="AZ8">
-        <v>85918</v>
+        <v>141270</v>
       </c>
       <c r="BA8">
         <v>52</v>
@@ -1956,10 +1956,10 @@
         <v>817</v>
       </c>
       <c r="BD8">
-        <v>1098</v>
+        <v>1236</v>
       </c>
       <c r="BE8">
-        <v>3559</v>
+        <v>5828</v>
       </c>
       <c r="BF8" t="b">
         <v>1</v>
@@ -2017,7 +2017,7 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q9">
-        <v>3658</v>
+        <v>3025</v>
       </c>
       <c r="R9">
         <v>50</v>
@@ -2051,46 +2051,46 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>3658</t>
+          <t>3025</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>254 x 146 x 43</t>
+          <t>457 x 191 x 74</t>
         </is>
       </c>
       <c r="AB9">
         <v>355</v>
       </c>
       <c r="AC9">
-        <v>3891</v>
+        <v>6717</v>
       </c>
       <c r="AD9">
-        <v>4322</v>
+        <v>22008</v>
       </c>
       <c r="AE9">
-        <v>0.95</v>
+        <v>0.55</v>
       </c>
       <c r="AF9">
         <v>0.21</v>
       </c>
       <c r="AG9">
-        <v>0.7</v>
+        <v>0.91</v>
       </c>
       <c r="AH9">
-        <v>2728</v>
+        <v>6093</v>
       </c>
       <c r="AI9">
         <v>355</v>
       </c>
       <c r="AJ9">
-        <v>3891</v>
+        <v>6717</v>
       </c>
       <c r="AK9">
-        <v>274000</v>
+        <v>473000</v>
       </c>
       <c r="AL9">
-        <v>181090</v>
+        <v>312611</v>
       </c>
       <c r="AM9">
         <v>0.15</v>
@@ -2102,37 +2102,37 @@
         <v>1.01</v>
       </c>
       <c r="AP9">
-        <v>3936</v>
+        <v>6795</v>
       </c>
       <c r="AQ9">
         <v>355</v>
       </c>
       <c r="AR9">
-        <v>1945</v>
+        <v>3358</v>
       </c>
       <c r="AS9">
-        <v>21924</v>
+        <v>54082</v>
       </c>
       <c r="AT9">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="AU9">
         <v>0.21</v>
       </c>
       <c r="AV9">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="AW9">
-        <v>1903</v>
+        <v>3322</v>
       </c>
       <c r="AX9">
-        <v>0.88</v>
+        <v>1.18</v>
       </c>
       <c r="AY9">
         <v>224223560</v>
       </c>
       <c r="AZ9">
-        <v>181090</v>
+        <v>312611</v>
       </c>
       <c r="BA9">
         <v>52</v>
@@ -2144,10 +2144,10 @@
         <v>206</v>
       </c>
       <c r="BD9">
-        <v>263</v>
+        <v>296</v>
       </c>
       <c r="BE9">
-        <v>1855</v>
+        <v>3055</v>
       </c>
       <c r="BF9" t="b">
         <v>1</v>
@@ -2205,7 +2205,7 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q10">
-        <v>3843</v>
+        <v>3356</v>
       </c>
       <c r="R10">
         <v>50</v>
@@ -2239,46 +2239,46 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>3843</t>
+          <t>3356</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>457 x 152 x 52</t>
+          <t>610 x 178 x 82</t>
         </is>
       </c>
       <c r="AB10">
         <v>355</v>
       </c>
       <c r="AC10">
-        <v>4729</v>
+        <v>7384</v>
       </c>
       <c r="AD10">
-        <v>3536</v>
+        <v>9236</v>
       </c>
       <c r="AE10">
-        <v>1.16</v>
+        <v>0.89</v>
       </c>
       <c r="AF10">
         <v>0.21</v>
       </c>
       <c r="AG10">
-        <v>0.5600000000000001</v>
+        <v>0.74</v>
       </c>
       <c r="AH10">
-        <v>2639</v>
+        <v>5448</v>
       </c>
       <c r="AI10">
         <v>355</v>
       </c>
       <c r="AJ10">
-        <v>4729</v>
+        <v>7384</v>
       </c>
       <c r="AK10">
-        <v>333000</v>
+        <v>520000</v>
       </c>
       <c r="AL10">
-        <v>63811</v>
+        <v>99645</v>
       </c>
       <c r="AM10">
         <v>0.27</v>
@@ -2290,37 +2290,37 @@
         <v>0.98</v>
       </c>
       <c r="AP10">
-        <v>4652</v>
+        <v>7265</v>
       </c>
       <c r="AQ10">
         <v>355</v>
       </c>
       <c r="AR10">
-        <v>2364</v>
+        <v>3692</v>
       </c>
       <c r="AS10">
-        <v>20888</v>
+        <v>39185</v>
       </c>
       <c r="AT10">
-        <v>0.34</v>
+        <v>0.31</v>
       </c>
       <c r="AU10">
         <v>0.21</v>
       </c>
       <c r="AV10">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="AW10">
-        <v>2291</v>
+        <v>3603</v>
       </c>
       <c r="AX10">
-        <v>0.97</v>
+        <v>1.26</v>
       </c>
       <c r="AY10">
         <v>224223560</v>
       </c>
       <c r="AZ10">
-        <v>55021</v>
+        <v>85918</v>
       </c>
       <c r="BA10">
         <v>52</v>
@@ -2332,10 +2332,10 @@
         <v>817</v>
       </c>
       <c r="BD10">
-        <v>994</v>
+        <v>1090</v>
       </c>
       <c r="BE10">
-        <v>2021</v>
+        <v>3465</v>
       </c>
       <c r="BF10" t="b">
         <v>1</v>
@@ -2393,7 +2393,7 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q11">
-        <v>2038</v>
+        <v>1780</v>
       </c>
       <c r="R11">
         <v>50</v>
@@ -2427,46 +2427,46 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>2038</t>
+          <t>1780</t>
         </is>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>254 x 102 x 25</t>
+          <t>305 x 127 x 42</t>
         </is>
       </c>
       <c r="AB11">
         <v>355</v>
       </c>
       <c r="AC11">
-        <v>2272</v>
+        <v>3791</v>
       </c>
       <c r="AD11">
-        <v>2254</v>
+        <v>5419</v>
       </c>
       <c r="AE11">
-        <v>1</v>
+        <v>0.84</v>
       </c>
       <c r="AF11">
         <v>0.21</v>
       </c>
       <c r="AG11">
-        <v>0.66</v>
+        <v>0.77</v>
       </c>
       <c r="AH11">
-        <v>1506</v>
+        <v>2935</v>
       </c>
       <c r="AI11">
         <v>355</v>
       </c>
       <c r="AJ11">
-        <v>2272</v>
+        <v>3791</v>
       </c>
       <c r="AK11">
-        <v>160000</v>
+        <v>267000</v>
       </c>
       <c r="AL11">
-        <v>105746</v>
+        <v>176463</v>
       </c>
       <c r="AM11">
         <v>0.15</v>
@@ -2478,52 +2478,52 @@
         <v>1.01</v>
       </c>
       <c r="AP11">
-        <v>2298</v>
+        <v>3835</v>
       </c>
       <c r="AQ11">
         <v>355</v>
       </c>
       <c r="AR11">
-        <v>1136</v>
+        <v>1896</v>
       </c>
       <c r="AS11">
-        <v>4825</v>
+        <v>12598</v>
       </c>
       <c r="AT11">
-        <v>0.49</v>
+        <v>0.39</v>
       </c>
       <c r="AU11">
         <v>0.21</v>
       </c>
       <c r="AV11">
-        <v>0.93</v>
+        <v>0.96</v>
       </c>
       <c r="AW11">
-        <v>1055</v>
+        <v>1812</v>
       </c>
       <c r="AX11">
-        <v>0.7</v>
+        <v>0.87</v>
       </c>
       <c r="AY11">
         <v>224223560</v>
       </c>
       <c r="AZ11">
-        <v>105746</v>
+        <v>176463</v>
       </c>
       <c r="BA11">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BB11">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="BC11">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="BD11">
-        <v>235</v>
+        <v>261</v>
       </c>
       <c r="BE11">
-        <v>1042</v>
+        <v>1806</v>
       </c>
       <c r="BF11" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
refine strut selection by sorting by mass, height and base (not only by mass)
</commit_message>
<xml_diff>
--- a/tables/input/output_processed_table.xlsx
+++ b/tables/input/output_processed_table.xlsx
@@ -701,10 +701,10 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q2">
-        <v>2915</v>
+        <v>4301</v>
       </c>
       <c r="R2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S2" t="inlineStr">
         <is>
@@ -730,51 +730,51 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>286</t>
+          <t>206</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>3202</t>
+          <t>4506</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>457 x 191 x 74</t>
+          <t>406 x 140 x 53</t>
         </is>
       </c>
       <c r="AB2">
         <v>355</v>
       </c>
       <c r="AC2">
-        <v>6717</v>
+        <v>4821</v>
       </c>
       <c r="AD2">
-        <v>5502</v>
+        <v>3024</v>
       </c>
       <c r="AE2">
-        <v>1.1</v>
+        <v>1.26</v>
       </c>
       <c r="AF2">
         <v>0.21</v>
       </c>
       <c r="AG2">
-        <v>0.59</v>
+        <v>0.49</v>
       </c>
       <c r="AH2">
-        <v>3981</v>
+        <v>2371</v>
       </c>
       <c r="AI2">
         <v>355</v>
       </c>
       <c r="AJ2">
-        <v>6717</v>
+        <v>4821</v>
       </c>
       <c r="AK2">
-        <v>473000</v>
+        <v>339500</v>
       </c>
       <c r="AL2">
-        <v>90639</v>
+        <v>65057</v>
       </c>
       <c r="AM2">
         <v>0.27</v>
@@ -786,52 +786,52 @@
         <v>0.98</v>
       </c>
       <c r="AP2">
-        <v>6608</v>
+        <v>4743</v>
       </c>
       <c r="AQ2">
         <v>355</v>
       </c>
       <c r="AR2">
-        <v>3358</v>
+        <v>2410</v>
       </c>
       <c r="AS2">
-        <v>54082</v>
+        <v>20564</v>
       </c>
       <c r="AT2">
-        <v>0.25</v>
+        <v>0.34</v>
       </c>
       <c r="AU2">
         <v>0.21</v>
       </c>
       <c r="AV2">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
       <c r="AW2">
-        <v>3322</v>
+        <v>2332</v>
       </c>
       <c r="AX2">
-        <v>1.18</v>
+        <v>0.98</v>
       </c>
       <c r="AY2">
         <v>224223560</v>
       </c>
       <c r="AZ2">
-        <v>78153</v>
+        <v>56095</v>
       </c>
       <c r="BA2">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="BB2">
-        <v>437</v>
+        <v>25</v>
       </c>
       <c r="BC2">
-        <v>817</v>
+        <v>47</v>
       </c>
       <c r="BD2">
-        <v>1085</v>
+        <v>357</v>
       </c>
       <c r="BE2">
-        <v>3310</v>
+        <v>2289</v>
       </c>
       <c r="BF2" t="b">
         <v>1</v>
@@ -889,10 +889,10 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q3">
-        <v>1546</v>
+        <v>4562</v>
       </c>
       <c r="R3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
@@ -918,51 +918,51 @@
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>208</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>1700</t>
+          <t>4770</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>305 x 165 x 40</t>
+          <t>406 x 178 x 54</t>
         </is>
       </c>
       <c r="AB3">
         <v>355</v>
       </c>
       <c r="AC3">
-        <v>3642</v>
+        <v>4899</v>
       </c>
       <c r="AD3">
-        <v>5618</v>
+        <v>12359</v>
       </c>
       <c r="AE3">
-        <v>0.8100000000000001</v>
+        <v>0.63</v>
       </c>
       <c r="AF3">
         <v>0.21</v>
       </c>
       <c r="AG3">
-        <v>0.79</v>
+        <v>0.88</v>
       </c>
       <c r="AH3">
-        <v>2887</v>
+        <v>4303</v>
       </c>
       <c r="AI3">
         <v>355</v>
       </c>
       <c r="AJ3">
-        <v>3642</v>
+        <v>4899</v>
       </c>
       <c r="AK3">
-        <v>256500</v>
+        <v>345000</v>
       </c>
       <c r="AL3">
-        <v>169524</v>
+        <v>228014</v>
       </c>
       <c r="AM3">
         <v>0.15</v>
@@ -974,16 +974,16 @@
         <v>1.01</v>
       </c>
       <c r="AP3">
-        <v>3685</v>
+        <v>4956</v>
       </c>
       <c r="AQ3">
         <v>355</v>
       </c>
       <c r="AR3">
-        <v>1821</v>
+        <v>2450</v>
       </c>
       <c r="AS3">
-        <v>24742</v>
+        <v>33032</v>
       </c>
       <c r="AT3">
         <v>0.27</v>
@@ -995,31 +995,31 @@
         <v>0.98</v>
       </c>
       <c r="AW3">
-        <v>1792</v>
+        <v>2410</v>
       </c>
       <c r="AX3">
-        <v>0.85</v>
+        <v>0.98</v>
       </c>
       <c r="AY3">
         <v>224223560</v>
       </c>
       <c r="AZ3">
-        <v>169524</v>
+        <v>228014</v>
       </c>
       <c r="BA3">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="BB3">
-        <v>218</v>
+        <v>13</v>
       </c>
       <c r="BC3">
-        <v>206</v>
+        <v>12</v>
       </c>
       <c r="BD3">
-        <v>259</v>
+        <v>152</v>
       </c>
       <c r="BE3">
-        <v>1726</v>
+        <v>2400</v>
       </c>
       <c r="BF3" t="b">
         <v>1</v>
@@ -1077,10 +1077,10 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q4">
-        <v>4810</v>
+        <v>7095</v>
       </c>
       <c r="R4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S4" t="inlineStr">
         <is>
@@ -1111,46 +1111,46 @@
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>4810</t>
+          <t>7095</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>610 x 229 x 113</t>
+          <t>533 x 210 x 82</t>
         </is>
       </c>
       <c r="AB4">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="AC4">
-        <v>9936</v>
+        <v>7455</v>
       </c>
       <c r="AD4">
-        <v>14424</v>
+        <v>7848</v>
       </c>
       <c r="AE4">
-        <v>0.83</v>
+        <v>0.97</v>
       </c>
       <c r="AF4">
         <v>0.21</v>
       </c>
       <c r="AG4">
-        <v>0.78</v>
+        <v>0.68</v>
       </c>
       <c r="AH4">
-        <v>7732</v>
+        <v>5094</v>
       </c>
       <c r="AI4">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="AJ4">
-        <v>9936</v>
+        <v>7455</v>
       </c>
       <c r="AK4">
-        <v>720000</v>
+        <v>525000</v>
       </c>
       <c r="AL4">
-        <v>137970</v>
+        <v>100603</v>
       </c>
       <c r="AM4">
         <v>0.27</v>
@@ -1162,52 +1162,52 @@
         <v>0.98</v>
       </c>
       <c r="AP4">
-        <v>9785</v>
+        <v>7335</v>
       </c>
       <c r="AQ4">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="AR4">
-        <v>4968</v>
+        <v>3728</v>
       </c>
       <c r="AS4">
-        <v>111079</v>
+        <v>65093</v>
       </c>
       <c r="AT4">
-        <v>0.21</v>
+        <v>0.24</v>
       </c>
       <c r="AU4">
         <v>0.21</v>
       </c>
       <c r="AV4">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="AW4">
-        <v>4955</v>
+        <v>3695</v>
       </c>
       <c r="AX4">
-        <v>1.56</v>
+        <v>1.26</v>
       </c>
       <c r="AY4">
         <v>224223560</v>
       </c>
       <c r="AZ4">
-        <v>118964</v>
+        <v>86745</v>
       </c>
       <c r="BA4">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="BB4">
-        <v>437</v>
+        <v>25</v>
       </c>
       <c r="BC4">
-        <v>817</v>
+        <v>47</v>
       </c>
       <c r="BD4">
-        <v>1182</v>
+        <v>531</v>
       </c>
       <c r="BE4">
-        <v>4928</v>
+        <v>3601</v>
       </c>
       <c r="BF4" t="b">
         <v>1</v>
@@ -1265,10 +1265,10 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q5">
-        <v>2551</v>
+        <v>7525</v>
       </c>
       <c r="R5">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S5" t="inlineStr">
         <is>
@@ -1299,46 +1299,46 @@
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>2551</t>
+          <t>7525</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>457 x 152 x 60</t>
+          <t>533 x 210 x 92</t>
         </is>
       </c>
       <c r="AB5">
         <v>355</v>
       </c>
       <c r="AC5">
-        <v>5410</v>
+        <v>8307</v>
       </c>
       <c r="AD5">
-        <v>16853</v>
+        <v>36482</v>
       </c>
       <c r="AE5">
-        <v>0.57</v>
+        <v>0.48</v>
       </c>
       <c r="AF5">
         <v>0.21</v>
       </c>
       <c r="AG5">
-        <v>0.9</v>
+        <v>0.93</v>
       </c>
       <c r="AH5">
-        <v>4881</v>
+        <v>7736</v>
       </c>
       <c r="AI5">
         <v>355</v>
       </c>
       <c r="AJ5">
-        <v>5410</v>
+        <v>8307</v>
       </c>
       <c r="AK5">
-        <v>381000</v>
+        <v>585000</v>
       </c>
       <c r="AL5">
-        <v>251807</v>
+        <v>386633</v>
       </c>
       <c r="AM5">
         <v>0.15</v>
@@ -1350,52 +1350,52 @@
         <v>1.01</v>
       </c>
       <c r="AP5">
-        <v>5473</v>
+        <v>8403</v>
       </c>
       <c r="AQ5">
         <v>355</v>
       </c>
       <c r="AR5">
-        <v>2705</v>
+        <v>4154</v>
       </c>
       <c r="AS5">
-        <v>25746</v>
+        <v>77399</v>
       </c>
       <c r="AT5">
-        <v>0.32</v>
+        <v>0.23</v>
       </c>
       <c r="AU5">
         <v>0.21</v>
       </c>
       <c r="AV5">
-        <v>0.97</v>
+        <v>0.99</v>
       </c>
       <c r="AW5">
-        <v>2629</v>
+        <v>4125</v>
       </c>
       <c r="AX5">
-        <v>1.04</v>
+        <v>1.36</v>
       </c>
       <c r="AY5">
         <v>224223560</v>
       </c>
       <c r="AZ5">
-        <v>251807</v>
+        <v>386633</v>
       </c>
       <c r="BA5">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="BB5">
-        <v>218</v>
+        <v>13</v>
       </c>
       <c r="BC5">
-        <v>206</v>
+        <v>12</v>
       </c>
       <c r="BD5">
-        <v>283</v>
+        <v>232</v>
       </c>
       <c r="BE5">
-        <v>2579</v>
+        <v>3786</v>
       </c>
       <c r="BF5" t="b">
         <v>1</v>
@@ -1453,10 +1453,10 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q6">
-        <v>6885</v>
+        <v>10164</v>
       </c>
       <c r="R6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
@@ -1487,46 +1487,46 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>6885</t>
+          <t>10164</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>457 x 191 x 161</t>
+          <t>610 x 229 x 125</t>
         </is>
       </c>
       <c r="AB6">
         <v>345</v>
       </c>
       <c r="AC6">
-        <v>14214</v>
+        <v>10971</v>
       </c>
       <c r="AD6">
-        <v>13185</v>
+        <v>16291</v>
       </c>
       <c r="AE6">
-        <v>1.04</v>
+        <v>0.82</v>
       </c>
       <c r="AF6">
         <v>0.21</v>
       </c>
       <c r="AG6">
-        <v>0.64</v>
+        <v>0.78</v>
       </c>
       <c r="AH6">
-        <v>9080</v>
+        <v>8598</v>
       </c>
       <c r="AI6">
         <v>345</v>
       </c>
       <c r="AJ6">
-        <v>14214</v>
+        <v>10971</v>
       </c>
       <c r="AK6">
-        <v>1030000</v>
+        <v>795000</v>
       </c>
       <c r="AL6">
-        <v>197374</v>
+        <v>152342</v>
       </c>
       <c r="AM6">
         <v>0.27</v>
@@ -1538,52 +1538,52 @@
         <v>0.98</v>
       </c>
       <c r="AP6">
-        <v>13998</v>
+        <v>10804</v>
       </c>
       <c r="AQ6">
         <v>345</v>
       </c>
       <c r="AR6">
-        <v>7107</v>
+        <v>5486</v>
       </c>
       <c r="AS6">
-        <v>137635</v>
+        <v>127272</v>
       </c>
       <c r="AT6">
-        <v>0.23</v>
+        <v>0.21</v>
       </c>
       <c r="AU6">
         <v>0.21</v>
       </c>
       <c r="AV6">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="AW6">
-        <v>7064</v>
+        <v>5476</v>
       </c>
       <c r="AX6">
-        <v>2.03</v>
+        <v>1.68</v>
       </c>
       <c r="AY6">
         <v>224223560</v>
       </c>
       <c r="AZ6">
-        <v>170185</v>
+        <v>131356</v>
       </c>
       <c r="BA6">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="BB6">
-        <v>445</v>
+        <v>34</v>
       </c>
       <c r="BC6">
-        <v>833</v>
+        <v>63</v>
       </c>
       <c r="BD6">
-        <v>1326</v>
+        <v>748</v>
       </c>
       <c r="BE6">
-        <v>7018</v>
+        <v>5157</v>
       </c>
       <c r="BF6" t="b">
         <v>1</v>
@@ -1641,10 +1641,10 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q7">
-        <v>3651</v>
+        <v>10781</v>
       </c>
       <c r="R7">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S7" t="inlineStr">
         <is>
@@ -1675,49 +1675,49 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>3651</t>
+          <t>10781</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>533 x 210 x 82</t>
+          <t>686 x 254 x 125</t>
         </is>
       </c>
       <c r="AB7">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AC7">
-        <v>7455</v>
+        <v>10971</v>
       </c>
       <c r="AD7">
-        <v>31393</v>
+        <v>77987</v>
       </c>
       <c r="AE7">
-        <v>0.49</v>
+        <v>0.38</v>
       </c>
       <c r="AF7">
         <v>0.21</v>
       </c>
       <c r="AG7">
-        <v>0.93</v>
+        <v>0.96</v>
       </c>
       <c r="AH7">
-        <v>6919</v>
+        <v>10524</v>
       </c>
       <c r="AI7">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AJ7">
-        <v>7455</v>
+        <v>10971</v>
       </c>
       <c r="AK7">
-        <v>525000</v>
+        <v>795000</v>
       </c>
       <c r="AL7">
-        <v>346978</v>
+        <v>525424</v>
       </c>
       <c r="AM7">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="AN7">
         <v>0.21</v>
@@ -1726,52 +1726,52 @@
         <v>1.01</v>
       </c>
       <c r="AP7">
-        <v>7541</v>
+        <v>11103</v>
       </c>
       <c r="AQ7">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AR7">
-        <v>3728</v>
+        <v>5486</v>
       </c>
       <c r="AS7">
-        <v>65093</v>
+        <v>141845</v>
       </c>
       <c r="AT7">
-        <v>0.24</v>
+        <v>0.2</v>
       </c>
       <c r="AU7">
         <v>0.21</v>
       </c>
       <c r="AV7">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="AW7">
-        <v>3695</v>
+        <v>5490</v>
       </c>
       <c r="AX7">
-        <v>1.26</v>
+        <v>1.68</v>
       </c>
       <c r="AY7">
         <v>224223560</v>
       </c>
       <c r="AZ7">
-        <v>346978</v>
+        <v>525424</v>
       </c>
       <c r="BA7">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="BB7">
-        <v>218</v>
+        <v>17</v>
       </c>
       <c r="BC7">
-        <v>206</v>
+        <v>16</v>
       </c>
       <c r="BD7">
-        <v>315</v>
+        <v>332</v>
       </c>
       <c r="BE7">
-        <v>3682</v>
+        <v>5424</v>
       </c>
       <c r="BF7" t="b">
         <v>1</v>
@@ -1829,10 +1829,10 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q8">
-        <v>5704</v>
+        <v>8425</v>
       </c>
       <c r="R8">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
@@ -1863,46 +1863,46 @@
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>5704</t>
+          <t>8425</t>
         </is>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>762 x 267 x 134</t>
+          <t>457 x 191 x 98</t>
         </is>
       </c>
       <c r="AB8">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AC8">
-        <v>12141</v>
+        <v>8625</v>
       </c>
       <c r="AD8">
-        <v>24949</v>
+        <v>7551</v>
       </c>
       <c r="AE8">
-        <v>0.7</v>
+        <v>1.07</v>
       </c>
       <c r="AF8">
         <v>0.21</v>
       </c>
       <c r="AG8">
-        <v>0.85</v>
+        <v>0.62</v>
       </c>
       <c r="AH8">
-        <v>10306</v>
+        <v>5326</v>
       </c>
       <c r="AI8">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AJ8">
-        <v>12141</v>
+        <v>8625</v>
       </c>
       <c r="AK8">
-        <v>855000</v>
+        <v>625000</v>
       </c>
       <c r="AL8">
-        <v>163839</v>
+        <v>119766</v>
       </c>
       <c r="AM8">
         <v>0.27</v>
@@ -1914,52 +1914,52 @@
         <v>0.98</v>
       </c>
       <c r="AP8">
-        <v>11946</v>
+        <v>8494</v>
       </c>
       <c r="AQ8">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AR8">
-        <v>6070</v>
+        <v>4312</v>
       </c>
       <c r="AS8">
-        <v>155122</v>
+        <v>76104</v>
       </c>
       <c r="AT8">
-        <v>0.2</v>
+        <v>0.24</v>
       </c>
       <c r="AU8">
         <v>0.21</v>
       </c>
       <c r="AV8">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="AW8">
-        <v>6073</v>
+        <v>4276</v>
       </c>
       <c r="AX8">
-        <v>1.77</v>
+        <v>1.42</v>
       </c>
       <c r="AY8">
         <v>224223560</v>
       </c>
       <c r="AZ8">
-        <v>141270</v>
+        <v>103267</v>
       </c>
       <c r="BA8">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="BB8">
-        <v>437</v>
+        <v>25</v>
       </c>
       <c r="BC8">
-        <v>817</v>
+        <v>47</v>
       </c>
       <c r="BD8">
-        <v>1236</v>
+        <v>620</v>
       </c>
       <c r="BE8">
-        <v>5828</v>
+        <v>4274</v>
       </c>
       <c r="BF8" t="b">
         <v>1</v>
@@ -2017,10 +2017,10 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q9">
-        <v>3025</v>
+        <v>8936</v>
       </c>
       <c r="R9">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
@@ -2051,25 +2051,25 @@
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>3025</t>
+          <t>8936</t>
         </is>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>457 x 191 x 74</t>
+          <t>457 x 191 x 106</t>
         </is>
       </c>
       <c r="AB9">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AC9">
-        <v>6717</v>
+        <v>9315</v>
       </c>
       <c r="AD9">
-        <v>22008</v>
+        <v>32319</v>
       </c>
       <c r="AE9">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="AF9">
         <v>0.21</v>
@@ -2078,22 +2078,22 @@
         <v>0.91</v>
       </c>
       <c r="AH9">
-        <v>6093</v>
+        <v>8499</v>
       </c>
       <c r="AI9">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AJ9">
-        <v>6717</v>
+        <v>9315</v>
       </c>
       <c r="AK9">
-        <v>473000</v>
+        <v>675000</v>
       </c>
       <c r="AL9">
-        <v>312611</v>
+        <v>446115</v>
       </c>
       <c r="AM9">
-        <v>0.15</v>
+        <v>0.14</v>
       </c>
       <c r="AN9">
         <v>0.21</v>
@@ -2102,19 +2102,19 @@
         <v>1.01</v>
       </c>
       <c r="AP9">
-        <v>6795</v>
+        <v>9427</v>
       </c>
       <c r="AQ9">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="AR9">
-        <v>3358</v>
+        <v>4658</v>
       </c>
       <c r="AS9">
-        <v>54082</v>
+        <v>81285</v>
       </c>
       <c r="AT9">
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="AU9">
         <v>0.21</v>
@@ -2123,31 +2123,31 @@
         <v>0.99</v>
       </c>
       <c r="AW9">
-        <v>3322</v>
+        <v>4617</v>
       </c>
       <c r="AX9">
-        <v>1.18</v>
+        <v>1.49</v>
       </c>
       <c r="AY9">
         <v>224223560</v>
       </c>
       <c r="AZ9">
-        <v>312611</v>
+        <v>446115</v>
       </c>
       <c r="BA9">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="BB9">
-        <v>218</v>
+        <v>17</v>
       </c>
       <c r="BC9">
-        <v>206</v>
+        <v>16</v>
       </c>
       <c r="BD9">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="BE9">
-        <v>3055</v>
+        <v>4496</v>
       </c>
       <c r="BF9" t="b">
         <v>1</v>
@@ -2205,10 +2205,10 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q10">
-        <v>3356</v>
+        <v>4953</v>
       </c>
       <c r="R10">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
@@ -2239,46 +2239,46 @@
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>3356</t>
+          <t>4953</t>
         </is>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
-          <t>610 x 178 x 82</t>
+          <t>457 x 152 x 60</t>
         </is>
       </c>
       <c r="AB10">
         <v>355</v>
       </c>
       <c r="AC10">
-        <v>7384</v>
+        <v>5410</v>
       </c>
       <c r="AD10">
-        <v>9236</v>
+        <v>4213</v>
       </c>
       <c r="AE10">
-        <v>0.89</v>
+        <v>1.13</v>
       </c>
       <c r="AF10">
         <v>0.21</v>
       </c>
       <c r="AG10">
-        <v>0.74</v>
+        <v>0.57</v>
       </c>
       <c r="AH10">
-        <v>5448</v>
+        <v>3103</v>
       </c>
       <c r="AI10">
         <v>355</v>
       </c>
       <c r="AJ10">
-        <v>7384</v>
+        <v>5410</v>
       </c>
       <c r="AK10">
-        <v>520000</v>
+        <v>381000</v>
       </c>
       <c r="AL10">
-        <v>99645</v>
+        <v>73009</v>
       </c>
       <c r="AM10">
         <v>0.27</v>
@@ -2290,52 +2290,52 @@
         <v>0.98</v>
       </c>
       <c r="AP10">
-        <v>7265</v>
+        <v>5323</v>
       </c>
       <c r="AQ10">
         <v>355</v>
       </c>
       <c r="AR10">
-        <v>3692</v>
+        <v>2705</v>
       </c>
       <c r="AS10">
-        <v>39185</v>
+        <v>25746</v>
       </c>
       <c r="AT10">
-        <v>0.31</v>
+        <v>0.32</v>
       </c>
       <c r="AU10">
         <v>0.21</v>
       </c>
       <c r="AV10">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
       <c r="AW10">
-        <v>3603</v>
+        <v>2629</v>
       </c>
       <c r="AX10">
-        <v>1.26</v>
+        <v>1.04</v>
       </c>
       <c r="AY10">
         <v>224223560</v>
       </c>
       <c r="AZ10">
-        <v>85918</v>
+        <v>62952</v>
       </c>
       <c r="BA10">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="BB10">
-        <v>437</v>
+        <v>25</v>
       </c>
       <c r="BC10">
-        <v>817</v>
+        <v>47</v>
       </c>
       <c r="BD10">
-        <v>1090</v>
+        <v>385</v>
       </c>
       <c r="BE10">
-        <v>3465</v>
+        <v>2515</v>
       </c>
       <c r="BF10" t="b">
         <v>1</v>
@@ -2393,10 +2393,10 @@
         <v>9.630000000000001</v>
       </c>
       <c r="Q11">
-        <v>1780</v>
+        <v>5254</v>
       </c>
       <c r="R11">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
@@ -2427,46 +2427,46 @@
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>1780</t>
+          <t>5254</t>
         </is>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>305 x 127 x 42</t>
+          <t>533 x 165 x 66</t>
         </is>
       </c>
       <c r="AB11">
         <v>355</v>
       </c>
       <c r="AC11">
-        <v>3791</v>
+        <v>5943</v>
       </c>
       <c r="AD11">
-        <v>5419</v>
+        <v>23132</v>
       </c>
       <c r="AE11">
-        <v>0.84</v>
+        <v>0.51</v>
       </c>
       <c r="AF11">
         <v>0.21</v>
       </c>
       <c r="AG11">
-        <v>0.77</v>
+        <v>0.92</v>
       </c>
       <c r="AH11">
-        <v>2935</v>
+        <v>5480</v>
       </c>
       <c r="AI11">
         <v>355</v>
       </c>
       <c r="AJ11">
-        <v>3791</v>
+        <v>5943</v>
       </c>
       <c r="AK11">
-        <v>267000</v>
+        <v>418500</v>
       </c>
       <c r="AL11">
-        <v>176463</v>
+        <v>276591</v>
       </c>
       <c r="AM11">
         <v>0.15</v>
@@ -2478,52 +2478,52 @@
         <v>1.01</v>
       </c>
       <c r="AP11">
-        <v>3835</v>
+        <v>6012</v>
       </c>
       <c r="AQ11">
         <v>355</v>
       </c>
       <c r="AR11">
-        <v>1896</v>
+        <v>2971</v>
       </c>
       <c r="AS11">
-        <v>12598</v>
+        <v>27818</v>
       </c>
       <c r="AT11">
-        <v>0.39</v>
+        <v>0.33</v>
       </c>
       <c r="AU11">
         <v>0.21</v>
       </c>
       <c r="AV11">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="AW11">
-        <v>1812</v>
+        <v>2886</v>
       </c>
       <c r="AX11">
-        <v>0.87</v>
+        <v>1.1</v>
       </c>
       <c r="AY11">
         <v>224223560</v>
       </c>
       <c r="AZ11">
-        <v>176463</v>
+        <v>276591</v>
       </c>
       <c r="BA11">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="BB11">
-        <v>218</v>
+        <v>13</v>
       </c>
       <c r="BC11">
-        <v>206</v>
+        <v>12</v>
       </c>
       <c r="BD11">
-        <v>261</v>
+        <v>165</v>
       </c>
       <c r="BE11">
-        <v>1806</v>
+        <v>2644</v>
       </c>
       <c r="BF11" t="b">
         <v>1</v>

</xml_diff>